<commit_message>
Update Base Dwelling numbers
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35963459-CA74-4BFA-A761-F81A1CBD2DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0147D46D-96DE-4094-950C-7040DEF924A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{792F19A4-F3C1-4060-A832-2941269350EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1306,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5461D6A9-7CA5-4325-867E-528A650F94B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,7 +1355,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67D43401-6975-4CA9-A65A-90EF5B8A8F54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1405,7 +1405,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FAB907B-9BC9-4178-9F84-712BE42968BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1455,7 +1455,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794404CF-18CA-4F08-BF21-7F6289AD5541}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1504,7 +1504,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2046A1-69C1-440E-B2EB-7E1744F60DEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1880,7 +1880,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
@@ -12239,8 +12239,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:AQ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13399,7 +13399,7 @@
         <v>53</v>
       </c>
       <c r="J34" s="1">
-        <v>206.79888500000001</v>
+        <v>211.79900000000001</v>
       </c>
       <c r="K34" s="1">
         <v>227.33367966704699</v>
@@ -13515,7 +13515,7 @@
         <v>55</v>
       </c>
       <c r="J35" s="1">
-        <v>766.351721</v>
+        <v>788.10400000000004</v>
       </c>
       <c r="K35" s="1">
         <v>805.70916346620595</v>
@@ -13631,7 +13631,7 @@
         <v>57</v>
       </c>
       <c r="J36" s="1">
-        <v>724.42972899999995</v>
+        <v>735.43899999999996</v>
       </c>
       <c r="K36" s="1">
         <v>756.93265686674704</v>

</xml_diff>

<commit_message>
Add ILED paper scenario definitions and update LED Demands
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35963459-CA74-4BFA-A761-F81A1CBD2DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE909822-F270-4947-8DA0-5755BBF92A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7830" yWindow="-15855" windowWidth="21600" windowHeight="12405" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{792F19A4-F3C1-4060-A832-2941269350EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1306,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5461D6A9-7CA5-4325-867E-528A650F94B6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1355,7 +1355,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67D43401-6975-4CA9-A65A-90EF5B8A8F54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1405,7 +1405,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FAB907B-9BC9-4178-9F84-712BE42968BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1455,7 +1455,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794404CF-18CA-4F08-BF21-7F6289AD5541}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1504,7 +1504,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE2046A1-69C1-440E-B2EB-7E1744F60DEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1880,25 +1880,25 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:D24"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="3" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" style="3" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" style="3" customWidth="1"/>
     <col min="13" max="13" width="10" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="3"/>
+    <col min="14" max="14" width="11.3984375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.86328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1926,7 +1926,7 @@
       <c r="Y1" s="41"/>
       <c r="Z1" s="41"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1954,7 +1954,7 @@
       <c r="Y2" s="41"/>
       <c r="Z2" s="41"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1982,7 +1982,7 @@
       <c r="Y3" s="41"/>
       <c r="Z3" s="41"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -2010,7 +2010,7 @@
       <c r="Y4" s="41"/>
       <c r="Z4" s="41"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -2038,7 +2038,7 @@
       <c r="Y5" s="41"/>
       <c r="Z5" s="41"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="40"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
@@ -2066,7 +2066,7 @@
       <c r="Y6" s="41"/>
       <c r="Z6" s="41"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
@@ -2094,7 +2094,7 @@
       <c r="Y7" s="41"/>
       <c r="Z7" s="41"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
@@ -2122,7 +2122,7 @@
       <c r="Y8" s="41"/>
       <c r="Z8" s="41"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
@@ -2150,7 +2150,7 @@
       <c r="Y9" s="41"/>
       <c r="Z9" s="41"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
@@ -2178,7 +2178,7 @@
       <c r="Y10" s="41"/>
       <c r="Z10" s="41"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="40"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -2206,7 +2206,7 @@
       <c r="Y11" s="41"/>
       <c r="Z11" s="41"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -2234,7 +2234,7 @@
       <c r="Y12" s="41"/>
       <c r="Z12" s="41"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="40"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -2262,7 +2262,7 @@
       <c r="Y13" s="41"/>
       <c r="Z13" s="41"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="40"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
@@ -2290,7 +2290,7 @@
       <c r="Y14" s="41"/>
       <c r="Z14" s="41"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
@@ -2318,7 +2318,7 @@
       <c r="Y15" s="41"/>
       <c r="Z15" s="41"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="56" t="s">
         <v>187</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="Y16" s="41"/>
       <c r="Z16" s="41"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -2376,7 +2376,7 @@
       <c r="Y17" s="41"/>
       <c r="Z17" s="41"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -2404,7 +2404,7 @@
       <c r="Y18" s="41"/>
       <c r="Z18" s="41"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="47" t="s">
         <v>188</v>
       </c>
@@ -2436,7 +2436,7 @@
       <c r="Y19" s="41"/>
       <c r="Z19" s="41"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="47" t="s">
         <v>189</v>
       </c>
@@ -2468,7 +2468,7 @@
       <c r="Y20" s="41"/>
       <c r="Z20" s="41"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="47" t="s">
         <v>190</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="Y21" s="41"/>
       <c r="Z21" s="41"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="47"/>
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
@@ -2528,7 +2528,7 @@
       <c r="Y22" s="41"/>
       <c r="Z22" s="41"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="47" t="s">
         <v>191</v>
       </c>
@@ -2560,7 +2560,7 @@
       <c r="Y23" s="41"/>
       <c r="Z23" s="41"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="47"/>
       <c r="B24" s="55" t="s">
         <v>202</v>
@@ -2590,7 +2590,7 @@
       <c r="Y24" s="41"/>
       <c r="Z24" s="41"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="47"/>
       <c r="B25" s="50" t="s">
         <v>203</v>
@@ -2620,7 +2620,7 @@
       <c r="Y25" s="41"/>
       <c r="Z25" s="41"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="47" t="s">
         <v>192</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="Y26" s="41"/>
       <c r="Z26" s="41"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="47"/>
       <c r="B27" s="55" t="s">
         <v>202</v>
@@ -2682,7 +2682,7 @@
       <c r="Y27" s="41"/>
       <c r="Z27" s="41"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="47"/>
       <c r="B28" s="50" t="s">
         <v>203</v>
@@ -2712,7 +2712,7 @@
       <c r="Y28" s="41"/>
       <c r="Z28" s="41"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="47" t="s">
         <v>193</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="Y29" s="41"/>
       <c r="Z29" s="41"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="47" t="s">
         <v>194</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="Y30" s="41"/>
       <c r="Z30" s="41"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="47" t="s">
         <v>196</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="Y31" s="41"/>
       <c r="Z31" s="41"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="53"/>
       <c r="B32" s="54" t="s">
         <v>198</v>
@@ -2838,7 +2838,7 @@
       <c r="Y32" s="41"/>
       <c r="Z32" s="41"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="40"/>
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
@@ -2866,7 +2866,7 @@
       <c r="Y33" s="41"/>
       <c r="Z33" s="41"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="40"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -2894,7 +2894,7 @@
       <c r="Y34" s="41"/>
       <c r="Z34" s="41"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="40"/>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
@@ -2922,7 +2922,7 @@
       <c r="Y35" s="41"/>
       <c r="Z35" s="41"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="40"/>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
@@ -2950,7 +2950,7 @@
       <c r="Y36" s="41"/>
       <c r="Z36" s="41"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="40"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -2978,7 +2978,7 @@
       <c r="Y37" s="41"/>
       <c r="Z37" s="41"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="40"/>
       <c r="B38" s="40"/>
       <c r="C38" s="40"/>
@@ -3006,7 +3006,7 @@
       <c r="Y38" s="41"/>
       <c r="Z38" s="41"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="40"/>
       <c r="B39" s="40"/>
       <c r="C39" s="40"/>
@@ -3034,7 +3034,7 @@
       <c r="Y39" s="41"/>
       <c r="Z39" s="41"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
       <c r="C40" s="40"/>
@@ -3062,7 +3062,7 @@
       <c r="Y40" s="41"/>
       <c r="Z40" s="41"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="40"/>
       <c r="B41" s="40"/>
       <c r="C41" s="40"/>
@@ -3090,7 +3090,7 @@
       <c r="Y41" s="41"/>
       <c r="Z41" s="41"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="40"/>
       <c r="B42" s="40"/>
       <c r="C42" s="40"/>
@@ -3118,7 +3118,7 @@
       <c r="Y42" s="41"/>
       <c r="Z42" s="41"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="41"/>
       <c r="B43" s="41"/>
       <c r="C43" s="41"/>
@@ -3146,7 +3146,7 @@
       <c r="Y43" s="41"/>
       <c r="Z43" s="41"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="41"/>
       <c r="B44" s="41"/>
       <c r="C44" s="41"/>
@@ -3174,7 +3174,7 @@
       <c r="Y44" s="41"/>
       <c r="Z44" s="41"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="41"/>
       <c r="B45" s="41"/>
       <c r="C45" s="41"/>
@@ -3202,7 +3202,7 @@
       <c r="Y45" s="41"/>
       <c r="Z45" s="41"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="41"/>
       <c r="B46" s="41"/>
       <c r="C46" s="41"/>
@@ -3230,7 +3230,7 @@
       <c r="Y46" s="41"/>
       <c r="Z46" s="41"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="41"/>
       <c r="B47" s="41"/>
       <c r="C47" s="41"/>
@@ -3258,7 +3258,7 @@
       <c r="Y47" s="41"/>
       <c r="Z47" s="41"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="41"/>
       <c r="B48" s="41"/>
       <c r="C48" s="41"/>
@@ -3286,7 +3286,7 @@
       <c r="Y48" s="41"/>
       <c r="Z48" s="41"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="41"/>
       <c r="B49" s="41"/>
       <c r="C49" s="41"/>
@@ -3314,7 +3314,7 @@
       <c r="Y49" s="41"/>
       <c r="Z49" s="41"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -3342,7 +3342,7 @@
       <c r="Y50" s="41"/>
       <c r="Z50" s="41"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="41"/>
@@ -3370,7 +3370,7 @@
       <c r="Y51" s="41"/>
       <c r="Z51" s="41"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
       <c r="C52" s="41"/>
@@ -3398,7 +3398,7 @@
       <c r="Y52" s="41"/>
       <c r="Z52" s="41"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="41"/>
@@ -3426,7 +3426,7 @@
       <c r="Y53" s="41"/>
       <c r="Z53" s="41"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="41"/>
       <c r="B54" s="41"/>
       <c r="C54" s="41"/>
@@ -3454,7 +3454,7 @@
       <c r="Y54" s="41"/>
       <c r="Z54" s="41"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="41"/>
       <c r="B55" s="41"/>
       <c r="C55" s="41"/>
@@ -3482,7 +3482,7 @@
       <c r="Y55" s="41"/>
       <c r="Z55" s="41"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="41"/>
       <c r="B56" s="41"/>
       <c r="C56" s="41"/>
@@ -3510,7 +3510,7 @@
       <c r="Y56" s="41"/>
       <c r="Z56" s="41"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="41"/>
       <c r="B57" s="41"/>
       <c r="C57" s="41"/>
@@ -3538,7 +3538,7 @@
       <c r="Y57" s="41"/>
       <c r="Z57" s="41"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="41"/>
       <c r="B58" s="41"/>
       <c r="C58" s="41"/>
@@ -3566,7 +3566,7 @@
       <c r="Y58" s="41"/>
       <c r="Z58" s="41"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="41"/>
       <c r="B59" s="41"/>
       <c r="C59" s="41"/>
@@ -3594,7 +3594,7 @@
       <c r="Y59" s="41"/>
       <c r="Z59" s="41"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="41"/>
       <c r="B60" s="41"/>
       <c r="C60" s="41"/>
@@ -3622,7 +3622,7 @@
       <c r="Y60" s="41"/>
       <c r="Z60" s="41"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="41"/>
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
@@ -3650,7 +3650,7 @@
       <c r="Y61" s="41"/>
       <c r="Z61" s="41"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="41"/>
       <c r="B62" s="41"/>
       <c r="C62" s="41"/>
@@ -3678,7 +3678,7 @@
       <c r="Y62" s="41"/>
       <c r="Z62" s="41"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="41"/>
       <c r="B63" s="41"/>
       <c r="C63" s="41"/>
@@ -3706,7 +3706,7 @@
       <c r="Y63" s="41"/>
       <c r="Z63" s="41"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="41"/>
       <c r="B64" s="41"/>
       <c r="C64" s="41"/>
@@ -3734,7 +3734,7 @@
       <c r="Y64" s="41"/>
       <c r="Z64" s="41"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="41"/>
       <c r="B65" s="41"/>
       <c r="C65" s="41"/>
@@ -3762,7 +3762,7 @@
       <c r="Y65" s="41"/>
       <c r="Z65" s="41"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="41"/>
       <c r="B66" s="41"/>
       <c r="C66" s="41"/>
@@ -3790,7 +3790,7 @@
       <c r="Y66" s="41"/>
       <c r="Z66" s="41"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="41"/>
       <c r="B67" s="41"/>
       <c r="C67" s="41"/>
@@ -3818,7 +3818,7 @@
       <c r="Y67" s="41"/>
       <c r="Z67" s="41"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="41"/>
       <c r="B68" s="41"/>
       <c r="C68" s="41"/>
@@ -3846,7 +3846,7 @@
       <c r="Y68" s="41"/>
       <c r="Z68" s="41"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="41"/>
       <c r="B69" s="41"/>
       <c r="C69" s="41"/>
@@ -3874,7 +3874,7 @@
       <c r="Y69" s="41"/>
       <c r="Z69" s="41"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="41"/>
       <c r="B70" s="41"/>
       <c r="C70" s="41"/>
@@ -3902,7 +3902,7 @@
       <c r="Y70" s="41"/>
       <c r="Z70" s="41"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="41"/>
       <c r="B71" s="41"/>
       <c r="C71" s="41"/>
@@ -3930,7 +3930,7 @@
       <c r="Y71" s="41"/>
       <c r="Z71" s="41"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="41"/>
       <c r="B72" s="41"/>
       <c r="C72" s="41"/>
@@ -3958,7 +3958,7 @@
       <c r="Y72" s="41"/>
       <c r="Z72" s="41"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="41"/>
       <c r="B73" s="41"/>
       <c r="C73" s="41"/>
@@ -3986,7 +3986,7 @@
       <c r="Y73" s="41"/>
       <c r="Z73" s="41"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="41"/>
       <c r="B74" s="41"/>
       <c r="C74" s="41"/>
@@ -4014,7 +4014,7 @@
       <c r="Y74" s="41"/>
       <c r="Z74" s="41"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="41"/>
       <c r="B75" s="41"/>
       <c r="C75" s="41"/>
@@ -4042,7 +4042,7 @@
       <c r="Y75" s="41"/>
       <c r="Z75" s="41"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="41"/>
       <c r="B76" s="41"/>
       <c r="C76" s="41"/>
@@ -4070,7 +4070,7 @@
       <c r="Y76" s="41"/>
       <c r="Z76" s="41"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="41"/>
       <c r="B77" s="41"/>
       <c r="C77" s="41"/>
@@ -4098,7 +4098,7 @@
       <c r="Y77" s="41"/>
       <c r="Z77" s="41"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="41"/>
       <c r="B78" s="41"/>
       <c r="C78" s="41"/>
@@ -4126,7 +4126,7 @@
       <c r="Y78" s="41"/>
       <c r="Z78" s="41"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="41"/>
       <c r="B79" s="41"/>
       <c r="C79" s="41"/>
@@ -4154,7 +4154,7 @@
       <c r="Y79" s="41"/>
       <c r="Z79" s="41"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="41"/>
       <c r="B80" s="41"/>
       <c r="C80" s="41"/>
@@ -4182,7 +4182,7 @@
       <c r="Y80" s="41"/>
       <c r="Z80" s="41"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="41"/>
       <c r="B81" s="41"/>
       <c r="C81" s="41"/>
@@ -4210,7 +4210,7 @@
       <c r="Y81" s="41"/>
       <c r="Z81" s="41"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="41"/>
       <c r="B82" s="41"/>
       <c r="C82" s="41"/>
@@ -4238,7 +4238,7 @@
       <c r="Y82" s="41"/>
       <c r="Z82" s="41"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="41"/>
       <c r="B83" s="41"/>
       <c r="C83" s="41"/>
@@ -4266,7 +4266,7 @@
       <c r="Y83" s="41"/>
       <c r="Z83" s="41"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="41"/>
       <c r="B84" s="41"/>
       <c r="C84" s="41"/>
@@ -4294,7 +4294,7 @@
       <c r="Y84" s="41"/>
       <c r="Z84" s="41"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="41"/>
       <c r="B85" s="41"/>
       <c r="C85" s="41"/>
@@ -4322,7 +4322,7 @@
       <c r="Y85" s="41"/>
       <c r="Z85" s="41"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="41"/>
       <c r="B86" s="41"/>
       <c r="C86" s="41"/>
@@ -4350,7 +4350,7 @@
       <c r="Y86" s="41"/>
       <c r="Z86" s="41"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="41"/>
       <c r="B87" s="41"/>
       <c r="C87" s="41"/>
@@ -4378,7 +4378,7 @@
       <c r="Y87" s="41"/>
       <c r="Z87" s="41"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="41"/>
       <c r="B88" s="41"/>
       <c r="C88" s="41"/>
@@ -4406,7 +4406,7 @@
       <c r="Y88" s="41"/>
       <c r="Z88" s="41"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="41"/>
       <c r="B89" s="41"/>
       <c r="C89" s="41"/>
@@ -4434,7 +4434,7 @@
       <c r="Y89" s="41"/>
       <c r="Z89" s="41"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="41"/>
       <c r="B90" s="41"/>
       <c r="C90" s="41"/>
@@ -4462,7 +4462,7 @@
       <c r="Y90" s="41"/>
       <c r="Z90" s="41"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="41"/>
       <c r="B91" s="41"/>
       <c r="C91" s="41"/>
@@ -4490,7 +4490,7 @@
       <c r="Y91" s="41"/>
       <c r="Z91" s="41"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="41"/>
       <c r="B92" s="41"/>
       <c r="C92" s="41"/>
@@ -4518,7 +4518,7 @@
       <c r="Y92" s="41"/>
       <c r="Z92" s="41"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="41"/>
       <c r="B93" s="41"/>
       <c r="C93" s="41"/>
@@ -4546,7 +4546,7 @@
       <c r="Y93" s="41"/>
       <c r="Z93" s="41"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="41"/>
       <c r="B94" s="41"/>
       <c r="C94" s="41"/>
@@ -4574,7 +4574,7 @@
       <c r="Y94" s="41"/>
       <c r="Z94" s="41"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="41"/>
       <c r="B95" s="41"/>
       <c r="C95" s="41"/>
@@ -4602,7 +4602,7 @@
       <c r="Y95" s="41"/>
       <c r="Z95" s="41"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="41"/>
       <c r="B96" s="41"/>
       <c r="C96" s="41"/>
@@ -4630,7 +4630,7 @@
       <c r="Y96" s="41"/>
       <c r="Z96" s="41"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="41"/>
       <c r="B97" s="41"/>
       <c r="C97" s="41"/>
@@ -4658,7 +4658,7 @@
       <c r="Y97" s="41"/>
       <c r="Z97" s="41"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="41"/>
       <c r="B98" s="41"/>
       <c r="C98" s="41"/>
@@ -4686,7 +4686,7 @@
       <c r="Y98" s="41"/>
       <c r="Z98" s="41"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="41"/>
       <c r="B99" s="41"/>
       <c r="C99" s="41"/>
@@ -4745,21 +4745,21 @@
       <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="9" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="6" width="9.1328125" style="3"/>
+    <col min="7" max="7" width="10.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" style="3"/>
+    <col min="9" max="9" width="11.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:37" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C6" s="3" t="s">
         <v>66</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>0.20769618859639599</v>
       </c>
     </row>
-    <row r="7" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
         <v>66</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>0.47664625412085698</v>
       </c>
     </row>
-    <row r="8" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>0.42809298937083901</v>
       </c>
     </row>
-    <row r="9" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C9" s="3" t="s">
         <v>66</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>0.154582741264056</v>
       </c>
     </row>
-    <row r="10" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>9.95787628254481E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C11" s="3" t="s">
         <v>66</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="13" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C14" s="3" t="s">
         <v>66</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C15" s="3" t="s">
         <v>66</v>
       </c>
@@ -5834,7 +5834,7 @@
       <c r="AJ15" s="22"/>
       <c r="AK15" s="22"/>
     </row>
-    <row r="16" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C16" s="3" t="s">
         <v>66</v>
       </c>
@@ -5883,7 +5883,7 @@
       <c r="AJ16" s="22"/>
       <c r="AK16" s="22"/>
     </row>
-    <row r="17" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
@@ -5932,7 +5932,7 @@
       <c r="AJ17" s="22"/>
       <c r="AK17" s="22"/>
     </row>
-    <row r="18" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C18" s="3" t="s">
         <v>66</v>
       </c>
@@ -5981,7 +5981,7 @@
       <c r="AJ18" s="22"/>
       <c r="AK18" s="22"/>
     </row>
-    <row r="19" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C19" s="3" t="s">
         <v>66</v>
       </c>
@@ -6030,7 +6030,7 @@
       <c r="AJ19" s="22"/>
       <c r="AK19" s="22"/>
     </row>
-    <row r="20" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
@@ -6079,7 +6079,7 @@
       <c r="AJ20" s="22"/>
       <c r="AK20" s="22"/>
     </row>
-    <row r="21" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C21" s="3" t="s">
         <v>66</v>
       </c>
@@ -6128,7 +6128,7 @@
       <c r="AJ21" s="22"/>
       <c r="AK21" s="22"/>
     </row>
-    <row r="22" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C22" s="3" t="s">
         <v>66</v>
       </c>
@@ -6177,7 +6177,7 @@
       <c r="AJ22" s="22"/>
       <c r="AK22" s="22"/>
     </row>
-    <row r="23" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C23" s="3" t="s">
         <v>66</v>
       </c>
@@ -6226,7 +6226,7 @@
       <c r="AJ23" s="22"/>
       <c r="AK23" s="22"/>
     </row>
-    <row r="24" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C24" s="3" t="s">
         <v>66</v>
       </c>
@@ -6275,7 +6275,7 @@
       <c r="AJ24" s="22"/>
       <c r="AK24" s="22"/>
     </row>
-    <row r="25" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C25" s="3" t="s">
         <v>66</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="AJ25" s="22"/>
       <c r="AK25" s="22"/>
     </row>
-    <row r="26" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C26" s="3" t="s">
         <v>66</v>
       </c>
@@ -6373,7 +6373,7 @@
       <c r="AJ26" s="22"/>
       <c r="AK26" s="22"/>
     </row>
-    <row r="27" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C27" s="3" t="s">
         <v>66</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="AJ27" s="22"/>
       <c r="AK27" s="22"/>
     </row>
-    <row r="28" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C28" s="3" t="s">
         <v>66</v>
       </c>
@@ -6471,7 +6471,7 @@
       <c r="AJ28" s="22"/>
       <c r="AK28" s="22"/>
     </row>
-    <row r="29" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C29" s="3" t="s">
         <v>66</v>
       </c>
@@ -6520,7 +6520,7 @@
       <c r="AJ29" s="22"/>
       <c r="AK29" s="22"/>
     </row>
-    <row r="30" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C30" s="3" t="s">
         <v>66</v>
       </c>
@@ -6569,7 +6569,7 @@
       <c r="AJ30" s="22"/>
       <c r="AK30" s="22"/>
     </row>
-    <row r="31" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
@@ -6618,7 +6618,7 @@
       <c r="AJ31" s="22"/>
       <c r="AK31" s="22"/>
     </row>
-    <row r="32" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
@@ -6667,7 +6667,7 @@
       <c r="AJ32" s="22"/>
       <c r="AK32" s="22"/>
     </row>
-    <row r="33" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
@@ -6716,7 +6716,7 @@
       <c r="AJ33" s="22"/>
       <c r="AK33" s="22"/>
     </row>
-    <row r="34" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C34" s="3" t="s">
         <v>66</v>
       </c>
@@ -6765,7 +6765,7 @@
       <c r="AJ34" s="22"/>
       <c r="AK34" s="22"/>
     </row>
-    <row r="35" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C35" s="3" t="s">
         <v>66</v>
       </c>
@@ -6814,7 +6814,7 @@
       <c r="AJ35" s="22"/>
       <c r="AK35" s="22"/>
     </row>
-    <row r="36" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C36" s="3" t="s">
         <v>66</v>
       </c>
@@ -6863,7 +6863,7 @@
       <c r="AJ36" s="22"/>
       <c r="AK36" s="22"/>
     </row>
-    <row r="37" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C37" s="3" t="s">
         <v>66</v>
       </c>
@@ -6912,7 +6912,7 @@
       <c r="AJ37" s="22"/>
       <c r="AK37" s="22"/>
     </row>
-    <row r="38" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C38" s="3" t="s">
         <v>66</v>
       </c>
@@ -6961,7 +6961,7 @@
       <c r="AJ38" s="22"/>
       <c r="AK38" s="22"/>
     </row>
-    <row r="39" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C39" s="3" t="s">
         <v>66</v>
       </c>
@@ -7006,7 +7006,7 @@
       <c r="AJ39" s="22"/>
       <c r="AK39" s="22"/>
     </row>
-    <row r="40" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C40" s="3" t="s">
         <v>66</v>
       </c>
@@ -7051,7 +7051,7 @@
       <c r="AJ40" s="22"/>
       <c r="AK40" s="22"/>
     </row>
-    <row r="41" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C41" s="3" t="s">
         <v>66</v>
       </c>
@@ -7100,7 +7100,7 @@
       <c r="AJ41" s="22"/>
       <c r="AK41" s="22"/>
     </row>
-    <row r="42" spans="3:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:37" x14ac:dyDescent="0.45">
       <c r="C42" s="3" t="s">
         <v>66</v>
       </c>
@@ -7164,19 +7164,19 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.1328125" style="3"/>
+    <col min="4" max="4" width="11.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:32" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="13" t="s">
         <v>65</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:32" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D4" s="3" t="s">
         <v>59</v>
       </c>
@@ -7413,7 +7413,7 @@
         <v>0.2122596962048626</v>
       </c>
     </row>
-    <row r="5" spans="2:32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D5" s="3" t="s">
         <v>59</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>0.15354445783325901</v>
       </c>
     </row>
-    <row r="6" spans="2:32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:32" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D6" s="3" t="s">
         <v>59</v>
       </c>
@@ -7645,7 +7645,7 @@
         <v>0.23967972865007509</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D7" s="3" t="s">
         <v>59</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>0.26468469422110324</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D8" s="3" t="s">
         <v>59</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>0.48743823497682215</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>0.35260315962707711</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
@@ -8109,7 +8109,7 @@
         <v>0.45747736907548092</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>0.45737466284626727</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
@@ -8341,7 +8341,7 @@
         <v>0.43424277040967463</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D13" s="3" t="s">
         <v>59</v>
       </c>
@@ -8457,7 +8457,7 @@
         <v>0.31412261464919838</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D14" s="3" t="s">
         <v>59</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>0.4079856816277293</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D15" s="3" t="s">
         <v>59</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>0.40689805832883513</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.45">
       <c r="D16" s="3" t="s">
         <v>59</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>0.18922217409036649</v>
       </c>
     </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>0.15629751581539669</v>
       </c>
     </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D18" s="3" t="s">
         <v>59</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>0.14608329496284322</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D19" s="3" t="s">
         <v>59</v>
       </c>
@@ -9153,7 +9153,7 @@
         <v>0.12565485325773626</v>
       </c>
     </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D20" s="3" t="s">
         <v>59</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>0.14086885317580392</v>
       </c>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D21" s="3" t="s">
         <v>59</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>0.12806259379618537</v>
       </c>
     </row>
-    <row r="22" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
@@ -9499,7 +9499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D24" s="3" t="s">
         <v>59</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>5.5388643974572375E-2</v>
       </c>
     </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D25" s="3" t="s">
         <v>59</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>5.6842758875006623E-2</v>
       </c>
     </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D26" s="3" t="s">
         <v>59</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>5.2992018186097681E-2</v>
       </c>
     </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D27" s="3" t="s">
         <v>59</v>
       </c>
@@ -10075,7 +10075,7 @@
         <v>4.529053680827979E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>0.17571155329873456</v>
       </c>
     </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D29" s="3" t="s">
         <v>59</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>0.17505912318297531</v>
       </c>
     </row>
-    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D30" s="3" t="s">
         <v>59</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D31" s="3" t="s">
         <v>59</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D32" s="3" t="s">
         <v>59</v>
       </c>
@@ -10655,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D33" s="3" t="s">
         <v>59</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D34" s="3" t="s">
         <v>59</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D35" s="3" t="s">
         <v>59</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D36" s="3" t="s">
         <v>59</v>
       </c>
@@ -11116,7 +11116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D37" s="3" t="s">
         <v>59</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D38" s="3" t="s">
         <v>59</v>
       </c>
@@ -11348,7 +11348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:32" x14ac:dyDescent="0.45">
       <c r="D39" s="3" t="s">
         <v>59</v>
       </c>
@@ -11478,38 +11478,38 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.59765625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="6.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1328125" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="3"/>
+    <col min="29" max="29" width="5.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="C3" s="19" t="str">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -11623,12 +11623,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>133</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>132</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>131</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="18" t="s">
         <v>130</v>
       </c>
@@ -11985,7 +11985,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
         <v>76</v>
       </c>
@@ -11993,7 +11993,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>99</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>88</v>
       </c>
@@ -12009,7 +12009,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>89</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>100</v>
       </c>
@@ -12025,7 +12025,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>77</v>
       </c>
@@ -12033,7 +12033,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>94</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>90</v>
       </c>
@@ -12049,7 +12049,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>78</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>79</v>
       </c>
@@ -12065,7 +12065,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>80</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>95</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>91</v>
       </c>
@@ -12089,7 +12089,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>81</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>82</v>
       </c>
@@ -12105,7 +12105,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>96</v>
       </c>
@@ -12113,7 +12113,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>83</v>
       </c>
@@ -12121,7 +12121,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>101</v>
       </c>
@@ -12129,7 +12129,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>84</v>
       </c>
@@ -12137,7 +12137,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>97</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>98</v>
       </c>
@@ -12153,7 +12153,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>92</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>93</v>
       </c>
@@ -12169,7 +12169,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>85</v>
       </c>
@@ -12177,7 +12177,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>86</v>
       </c>
@@ -12185,7 +12185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>87</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>102</v>
       </c>
@@ -12239,23 +12239,23 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:AQ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AJ41" sqref="AJ41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.86328125" customWidth="1"/>
+    <col min="12" max="13" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.45">
       <c r="C1" t="s">
         <v>149</v>
       </c>
@@ -12263,7 +12263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12333,7 +12333,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D4" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12368,7 +12368,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12403,7 +12403,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12438,7 +12438,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D7" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12473,7 +12473,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D8" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12543,7 +12543,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D10" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12578,7 +12578,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D11" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D12" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12648,7 +12648,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D13" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12683,7 +12683,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D14" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12718,7 +12718,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D15" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12753,7 +12753,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D16" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -12788,7 +12788,7 @@
       </c>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -12823,7 +12823,7 @@
       </c>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -12858,7 +12858,7 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -12893,7 +12893,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -12929,7 +12929,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -12964,7 +12964,7 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -13001,7 +13001,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -13036,7 +13036,7 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -13073,7 +13073,7 @@
       </c>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -13110,7 +13110,7 @@
       </c>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -13144,7 +13144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -13178,7 +13178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -13207,7 +13207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.45">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -13236,19 +13236,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.45">
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.45">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>149</v>
       </c>
@@ -13260,7 +13260,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C33" s="13" t="s">
         <v>1</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="34" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:43" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
         <v>59</v>
       </c>
@@ -13467,11 +13467,11 @@
       <c r="AF34">
         <v>492.828423833106</v>
       </c>
-      <c r="AG34">
-        <v>502.36472594874499</v>
-      </c>
-      <c r="AH34">
-        <v>516.22001380752999</v>
+      <c r="AG34" s="3">
+        <v>496.36472594874499</v>
+      </c>
+      <c r="AH34" s="3">
+        <v>514.52001380752995</v>
       </c>
       <c r="AI34">
         <v>530.17405404626902</v>
@@ -13501,7 +13501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:43" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
         <v>59</v>
       </c>
@@ -13583,10 +13583,10 @@
       <c r="AF35">
         <v>1003.43540212397</v>
       </c>
-      <c r="AG35">
-        <v>1002.11497030569</v>
-      </c>
-      <c r="AH35">
+      <c r="AG35" s="3">
+        <v>1003.61497030569</v>
+      </c>
+      <c r="AH35" s="3">
         <v>1009.1830944926101</v>
       </c>
       <c r="AI35">
@@ -13617,7 +13617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:43" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
         <v>59</v>
       </c>
@@ -13699,11 +13699,11 @@
       <c r="AF36">
         <v>877.53441615506995</v>
       </c>
-      <c r="AG36">
-        <v>873.21565965240802</v>
-      </c>
-      <c r="AH36">
-        <v>876.17112006521802</v>
+      <c r="AG36" s="3">
+        <v>877.71565965240802</v>
+      </c>
+      <c r="AH36" s="3">
+        <v>877.87112006521807</v>
       </c>
       <c r="AI36">
         <v>878.89535131181003</v>
@@ -13733,25 +13733,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H40" s="36"/>
       <c r="I40" s="35"/>
       <c r="J40" s="35"/>
@@ -13759,7 +13759,7 @@
       <c r="L40" s="35"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H41" s="36"/>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
@@ -13767,7 +13767,7 @@
       <c r="L41" s="35"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="3:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:43" x14ac:dyDescent="0.45">
       <c r="H42" s="36"/>
       <c r="I42" s="35"/>
       <c r="J42" s="35"/>
@@ -13790,15 +13790,15 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.59765625" customWidth="1"/>
+    <col min="14" max="14" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C4" s="25" t="s">
         <v>150</v>
       </c>
@@ -13806,7 +13806,7 @@
       <c r="J4" s="26"/>
       <c r="K4" s="26"/>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C5" s="27" t="s">
         <v>65</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C6" s="28" t="s">
         <v>153</v>
       </c>
@@ -13856,7 +13856,7 @@
       <c r="L6" s="28"/>
       <c r="N6" s="30"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
       <c r="E7" t="s">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
       <c r="E8" t="s">
@@ -13908,7 +13908,7 @@
       </c>
       <c r="L8" s="29"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" t="s">
@@ -13934,7 +13934,7 @@
       </c>
       <c r="L9" s="29"/>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C10" s="29" t="s">
         <v>159</v>
       </c>
@@ -13962,7 +13962,7 @@
       </c>
       <c r="L10" s="29"/>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C11" s="29" t="s">
         <v>159</v>
       </c>
@@ -13990,7 +13990,7 @@
       </c>
       <c r="L11" s="29"/>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C12" s="29" t="s">
         <v>159</v>
       </c>
@@ -14018,7 +14018,7 @@
       </c>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" t="s">
@@ -14044,7 +14044,7 @@
       </c>
       <c r="L13" s="29"/>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="E14" t="s">
@@ -14070,7 +14070,7 @@
       </c>
       <c r="L14" s="29"/>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
       <c r="E15" t="s">
@@ -14096,7 +14096,7 @@
       </c>
       <c r="L15" s="29"/>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" t="s">
@@ -14122,7 +14122,7 @@
       </c>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" t="s">
@@ -14148,7 +14148,7 @@
       </c>
       <c r="L17" s="29"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" t="s">
@@ -14174,7 +14174,7 @@
       </c>
       <c r="L18" s="29"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" t="s">
@@ -14200,7 +14200,7 @@
       </c>
       <c r="L19" s="29"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
       <c r="E20" t="s">
@@ -14226,7 +14226,7 @@
       </c>
       <c r="L20" s="29"/>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" t="s">
@@ -14252,7 +14252,7 @@
       </c>
       <c r="L21" s="29"/>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E22" t="s">
         <v>154</v>
       </c>
@@ -14275,7 +14275,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E23" t="s">
         <v>154</v>
       </c>
@@ -14298,7 +14298,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E24" t="s">
         <v>154</v>
       </c>
@@ -14321,7 +14321,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>159</v>
       </c>
@@ -14347,7 +14347,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>159</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
         <v>159</v>
       </c>
@@ -14399,7 +14399,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
         <v>154</v>
       </c>
@@ -14422,7 +14422,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E29" t="s">
         <v>154</v>
       </c>
@@ -14445,7 +14445,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E30" t="s">
         <v>154</v>
       </c>
@@ -14468,7 +14468,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E31" t="s">
         <v>154</v>
       </c>
@@ -14491,7 +14491,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.45">
       <c r="E32" t="s">
         <v>154</v>
       </c>
@@ -14514,7 +14514,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E33" t="s">
         <v>154</v>
       </c>
@@ -14537,7 +14537,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E34" t="s">
         <v>154</v>
       </c>
@@ -14560,7 +14560,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E35" t="s">
         <v>154</v>
       </c>
@@ -14583,7 +14583,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E36" t="s">
         <v>154</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E37" t="s">
         <v>154</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E38" t="s">
         <v>154</v>
       </c>
@@ -14652,7 +14652,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E39" t="s">
         <v>154</v>
       </c>
@@ -14675,7 +14675,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E40" t="s">
         <v>154</v>
       </c>
@@ -14698,7 +14698,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E41" t="s">
         <v>154</v>
       </c>
@@ -14721,7 +14721,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E42" t="s">
         <v>154</v>
       </c>
@@ -14744,7 +14744,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E43" t="s">
         <v>154</v>
       </c>
@@ -14767,7 +14767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E44" t="s">
         <v>154</v>
       </c>
@@ -14790,7 +14790,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E45" t="s">
         <v>154</v>
       </c>
@@ -14813,7 +14813,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E46" t="s">
         <v>154</v>
       </c>
@@ -14836,7 +14836,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E47" t="s">
         <v>154</v>
       </c>
@@ -14859,7 +14859,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E48" t="s">
         <v>154</v>
       </c>
@@ -14882,7 +14882,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E49" t="s">
         <v>154</v>
       </c>
@@ -14905,7 +14905,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E50" t="s">
         <v>154</v>
       </c>
@@ -14928,7 +14928,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:11" x14ac:dyDescent="0.45">
       <c r="E51" t="s">
         <v>154</v>
       </c>
@@ -14965,18 +14965,18 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" customWidth="1"/>
+    <col min="11" max="11" width="12.3984375" customWidth="1"/>
+    <col min="12" max="12" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C3" s="25" t="s">
         <v>150</v>
       </c>
@@ -14984,7 +14984,7 @@
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
     </row>
-    <row r="4" spans="3:14" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" ht="29.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="27" t="s">
         <v>65</v>
       </c>
@@ -15017,7 +15017,7 @@
       </c>
       <c r="N4" s="34"/>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C5" s="28" t="s">
         <v>153</v>
       </c>
@@ -15033,7 +15033,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>154</v>
       </c>
@@ -15050,7 +15050,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E7" t="s">
         <v>154</v>
       </c>
@@ -15067,7 +15067,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E8" t="s">
         <v>154</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E9" t="s">
         <v>154</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E10" t="s">
         <v>154</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E11" t="s">
         <v>154</v>
       </c>
@@ -15135,7 +15135,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E12" t="s">
         <v>154</v>
       </c>
@@ -15152,7 +15152,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E13" t="s">
         <v>154</v>
       </c>
@@ -15169,7 +15169,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E14" t="s">
         <v>154</v>
       </c>
@@ -15186,7 +15186,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>154</v>
       </c>
@@ -15203,7 +15203,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>154</v>
       </c>
@@ -15220,7 +15220,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E17" t="s">
         <v>154</v>
       </c>
@@ -15237,7 +15237,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E18" t="s">
         <v>154</v>
       </c>
@@ -15254,7 +15254,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E19" t="s">
         <v>154</v>
       </c>
@@ -15271,7 +15271,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E20" t="s">
         <v>154</v>
       </c>
@@ -15288,7 +15288,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E21" t="s">
         <v>154</v>
       </c>
@@ -15305,7 +15305,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E22" t="s">
         <v>154</v>
       </c>
@@ -15322,7 +15322,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E23" t="s">
         <v>154</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E24" t="s">
         <v>154</v>
       </c>
@@ -15356,7 +15356,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E25" t="s">
         <v>154</v>
       </c>
@@ -15373,7 +15373,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E26" t="s">
         <v>154</v>
       </c>
@@ -15390,7 +15390,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E27" t="s">
         <v>154</v>
       </c>
@@ -15407,7 +15407,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
         <v>154</v>
       </c>
@@ -15424,7 +15424,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E29" t="s">
         <v>154</v>
       </c>
@@ -15441,7 +15441,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E30" t="s">
         <v>154</v>
       </c>
@@ -15458,7 +15458,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E31" t="s">
         <v>154</v>
       </c>
@@ -15475,7 +15475,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E32" t="s">
         <v>154</v>
       </c>
@@ -15492,7 +15492,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.45">
       <c r="E33" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
Update the 2018 building stock totals
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\veda-info-messages\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\update-rsd\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF13F204-5FC3-40D7-864E-1133C1199044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D811AEE-C4C1-4871-8E9B-972BB353FC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="0" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -5790,10 +5790,10 @@
         <v>68</v>
       </c>
       <c r="J15" s="20">
-        <v>1.1293662452688</v>
+        <v>1.1544546193487999</v>
       </c>
       <c r="K15" s="20">
-        <v>1.1293662452688</v>
+        <v>1.1544546193487999</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -5888,10 +5888,10 @@
         <v>70</v>
       </c>
       <c r="J17" s="20">
-        <v>0.77162665337257497</v>
+        <v>0.78876799986757495</v>
       </c>
       <c r="K17" s="20">
-        <v>0.77162665337257497</v>
+        <v>0.78876799986757495</v>
       </c>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
@@ -5937,10 +5937,10 @@
         <v>71</v>
       </c>
       <c r="J18" s="20">
-        <v>1.0288379823457801</v>
+        <v>1.05169316530962</v>
       </c>
       <c r="K18" s="20">
-        <v>1.0288379823457801</v>
+        <v>1.05169316530962</v>
       </c>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
@@ -5986,10 +5986,10 @@
         <v>72</v>
       </c>
       <c r="J19" s="20">
-        <v>0.83034086441921995</v>
+        <v>0.84878652127122001</v>
       </c>
       <c r="K19" s="20">
-        <v>0.83034086441921995</v>
+        <v>0.84878652127122001</v>
       </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -6133,10 +6133,10 @@
         <v>52</v>
       </c>
       <c r="J22" s="20">
-        <v>206.79888500000001</v>
+        <v>211.819885</v>
       </c>
       <c r="K22" s="20">
-        <v>206.79888500000001</v>
+        <v>211.819885</v>
       </c>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
@@ -6182,10 +6182,10 @@
         <v>54</v>
       </c>
       <c r="J23" s="20">
-        <v>766.351721</v>
+        <v>788.06472099999996</v>
       </c>
       <c r="K23" s="20">
-        <v>766.351721</v>
+        <v>788.06472099999996</v>
       </c>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
@@ -6231,10 +6231,10 @@
         <v>56</v>
       </c>
       <c r="J24" s="20">
-        <v>724.42972899999995</v>
+        <v>735.40672900000004</v>
       </c>
       <c r="K24" s="20">
-        <v>724.42972899999995</v>
+        <v>735.40672900000004</v>
       </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
@@ -13411,7 +13411,7 @@
       </c>
       <c r="J34" s="31">
         <f>VLOOKUP(H34,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>206.79888500000001</v>
+        <v>211.819885</v>
       </c>
       <c r="K34" s="1">
         <v>227.33367966704699</v>
@@ -13528,7 +13528,7 @@
       </c>
       <c r="J35" s="31">
         <f>VLOOKUP(H35,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>766.351721</v>
+        <v>788.06472099999996</v>
       </c>
       <c r="K35" s="1">
         <v>805.70916346620595</v>
@@ -13645,7 +13645,7 @@
       </c>
       <c r="J36" s="31">
         <f>VLOOKUP(H36,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>724.42972899999995</v>
+        <v>735.40672900000004</v>
       </c>
       <c r="K36" s="1">
         <v>756.93265686674704</v>

</xml_diff>

<commit_message>
Update DC electricity demand in 2020-2021 according to CSO
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\update-rsd\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D811AEE-C4C1-4871-8E9B-972BB353FC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E720B6E-E630-484F-B6DD-C97CE1C045D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -4732,7 +4732,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="C4:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -12232,8 +12232,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:AQ42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12282,12 +12282,15 @@
         <v>2020</v>
       </c>
       <c r="K2" s="12">
+        <v>2021</v>
+      </c>
+      <c r="L2" s="12">
         <v>2030</v>
       </c>
-      <c r="L2" s="12">
+      <c r="M2" s="12">
         <v>2050</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>186</v>
       </c>
     </row>
@@ -12315,14 +12318,14 @@
       <c r="J3" s="30">
         <v>1.81463172003468</v>
       </c>
-      <c r="K3" s="30">
-        <f>J3*2/3+L3/3</f>
+      <c r="L3" s="30">
+        <f>J3*2/3+M3/3</f>
         <v>1.23293489482708</v>
       </c>
-      <c r="L3" s="30">
+      <c r="M3" s="30">
         <v>6.9541244411880462E-2</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0</v>
       </c>
       <c r="P3" s="1"/>
@@ -12351,14 +12354,14 @@
       <c r="J4" s="30">
         <v>22.997393933436499</v>
       </c>
-      <c r="K4" s="30">
-        <f t="shared" ref="K4:K16" si="0">J4*2/3+L4/3</f>
+      <c r="L4" s="30">
+        <f>J4*2/3+M4/3</f>
         <v>21.564038456241871</v>
       </c>
-      <c r="L4" s="30">
+      <c r="M4" s="30">
         <v>18.697327501852616</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0</v>
       </c>
       <c r="P4" s="1"/>
@@ -12387,14 +12390,14 @@
       <c r="J5" s="30">
         <v>1.3579701788487999</v>
       </c>
-      <c r="K5" s="30">
-        <f t="shared" si="0"/>
+      <c r="L5" s="30">
+        <f>J5*2/3+M5/3</f>
         <v>1.8168912035156706</v>
       </c>
-      <c r="L5" s="30">
+      <c r="M5" s="30">
         <v>2.7347332528494115</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0</v>
       </c>
       <c r="P5" s="1"/>
@@ -12423,14 +12426,14 @@
       <c r="J6" s="30">
         <v>5.7274313907438001</v>
       </c>
-      <c r="K6" s="30">
-        <f t="shared" si="0"/>
+      <c r="L6" s="30">
+        <f>J6*2/3+M6/3</f>
         <v>5.2212845051183363</v>
       </c>
-      <c r="L6" s="30">
+      <c r="M6" s="30">
         <v>4.2089907338674086</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0</v>
       </c>
       <c r="P6" s="1"/>
@@ -12459,14 +12462,14 @@
       <c r="J7" s="30">
         <v>1.1453307514123801</v>
       </c>
-      <c r="K7" s="30">
-        <f t="shared" si="0"/>
+      <c r="L7" s="30">
+        <f>J7*2/3+M7/3</f>
         <v>1.1872938839576666</v>
       </c>
-      <c r="L7" s="30">
+      <c r="M7" s="30">
         <v>1.2712201490482398</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0</v>
       </c>
       <c r="P7" s="1"/>
@@ -12495,14 +12498,14 @@
       <c r="J8" s="30">
         <v>10.4827865863979</v>
       </c>
-      <c r="K8" s="30">
-        <f t="shared" si="0"/>
+      <c r="L8" s="30">
+        <f>J8*2/3+M8/3</f>
         <v>9.391476771293469</v>
       </c>
-      <c r="L8" s="30">
+      <c r="M8" s="30">
         <v>7.2088571410846098</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0</v>
       </c>
       <c r="P8" s="1"/>
@@ -12531,14 +12534,14 @@
       <c r="J9" s="30">
         <v>1.05400776614231</v>
       </c>
-      <c r="K9" s="30">
-        <f t="shared" si="0"/>
+      <c r="L9" s="30">
+        <f>J9*2/3+M9/3</f>
         <v>0.86541028956347699</v>
       </c>
-      <c r="L9" s="30">
+      <c r="M9" s="30">
         <v>0.48821533640581133</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0</v>
       </c>
       <c r="P9" s="1"/>
@@ -12567,14 +12570,14 @@
       <c r="J10" s="30">
         <v>16.2067419529189</v>
       </c>
-      <c r="K10" s="30">
-        <f t="shared" si="0"/>
+      <c r="L10" s="30">
+        <f>J10*2/3+M10/3</f>
         <v>13.7661776960718</v>
       </c>
-      <c r="L10" s="30">
+      <c r="M10" s="30">
         <v>8.8850491823775997</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0</v>
       </c>
       <c r="P10" s="1"/>
@@ -12603,14 +12606,14 @@
       <c r="J11" s="30">
         <v>17.9214706310973</v>
       </c>
-      <c r="K11" s="30">
-        <f t="shared" si="0"/>
+      <c r="L11" s="30">
+        <f>J11*2/3+M11/3</f>
         <v>15.932252704329224</v>
       </c>
-      <c r="L11" s="30">
+      <c r="M11" s="30">
         <v>11.953816850793071</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0</v>
       </c>
       <c r="P11" s="1"/>
@@ -12639,14 +12642,14 @@
       <c r="J12" s="30">
         <v>2.2861941894738802</v>
       </c>
-      <c r="K12" s="30">
-        <f t="shared" si="0"/>
+      <c r="L12" s="30">
+        <f>J12*2/3+M12/3</f>
         <v>1.8333550602163233</v>
       </c>
-      <c r="L12" s="30">
+      <c r="M12" s="30">
         <v>0.92767680170120992</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>0</v>
       </c>
       <c r="P12" s="1"/>
@@ -12675,14 +12678,14 @@
       <c r="J13" s="30">
         <v>5.7966251432017799</v>
       </c>
-      <c r="K13" s="30">
-        <f t="shared" si="0"/>
+      <c r="L13" s="30">
+        <f>J13*2/3+M13/3</f>
         <v>6.8655407588300337</v>
       </c>
-      <c r="L13" s="30">
+      <c r="M13" s="30">
         <v>9.0033719900865421</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0</v>
       </c>
       <c r="P13" s="1"/>
@@ -12711,14 +12714,14 @@
       <c r="J14" s="30">
         <v>0.19444424313328701</v>
       </c>
-      <c r="K14" s="30">
-        <f t="shared" si="0"/>
+      <c r="L14" s="30">
+        <f>J14*2/3+M14/3</f>
         <v>0.13734812058446252</v>
       </c>
-      <c r="L14" s="30">
+      <c r="M14" s="30">
         <v>2.3155875486813523E-2</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>0</v>
       </c>
       <c r="P14" s="1"/>
@@ -12747,14 +12750,14 @@
       <c r="J15" s="30">
         <v>4.5897245674903298</v>
       </c>
-      <c r="K15" s="30">
-        <f t="shared" si="0"/>
+      <c r="L15" s="30">
+        <f>J15*2/3+M15/3</f>
         <v>4.1809760165229068</v>
       </c>
-      <c r="L15" s="30">
+      <c r="M15" s="30">
         <v>3.3634789145880619</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>0</v>
       </c>
       <c r="P15" s="1"/>
@@ -12783,14 +12786,14 @@
       <c r="J16" s="30">
         <v>3.5251257971202601</v>
       </c>
-      <c r="K16" s="30">
-        <f t="shared" si="0"/>
+      <c r="L16" s="30">
+        <f>J16*2/3+M16/3</f>
         <v>3.4314725583947805</v>
       </c>
-      <c r="L16" s="30">
+      <c r="M16" s="30">
         <v>3.2441660809438213</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>0</v>
       </c>
       <c r="P16" s="1"/>
@@ -12819,13 +12822,13 @@
       <c r="J17" s="30">
         <v>10.76129175</v>
       </c>
-      <c r="K17" s="30">
+      <c r="L17" s="30">
         <v>16.798154247711324</v>
       </c>
-      <c r="L17" s="30">
+      <c r="M17" s="30">
         <v>18.550648173612263</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>0</v>
       </c>
       <c r="P17" s="1"/>
@@ -12854,13 +12857,13 @@
       <c r="J18" s="30">
         <v>23.13677727</v>
       </c>
-      <c r="K18" s="30">
+      <c r="L18" s="30">
         <v>30.018312954312446</v>
       </c>
-      <c r="L18" s="30">
+      <c r="M18" s="30">
         <v>30.011573675084005</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>0</v>
       </c>
       <c r="P18" s="1"/>
@@ -12889,13 +12892,13 @@
       <c r="J19" s="30">
         <v>19.908389740000001</v>
       </c>
-      <c r="K19" s="30">
+      <c r="L19" s="30">
         <v>25.857221286837778</v>
       </c>
-      <c r="L19" s="30">
+      <c r="M19" s="30">
         <v>25.788290151303741</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>0</v>
       </c>
       <c r="P19" s="1"/>
@@ -12924,14 +12927,14 @@
       <c r="J20" s="30">
         <v>11.754512350000001</v>
       </c>
-      <c r="K20" s="30">
-        <f t="shared" ref="K20:K25" si="1">(J20*2/3)+(L20/3)</f>
+      <c r="L20" s="30">
+        <f>(J20*2/3)+(M20/3)</f>
         <v>10.986341566666667</v>
       </c>
-      <c r="L20" s="30">
+      <c r="M20" s="30">
         <v>9.4499999999999993</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>0</v>
       </c>
       <c r="P20" s="1"/>
@@ -12960,13 +12963,13 @@
       <c r="J21" s="30">
         <v>9.9341345454545458</v>
       </c>
-      <c r="K21" s="30">
-        <v>0</v>
-      </c>
       <c r="L21" s="30">
         <v>0</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="30">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <v>0</v>
       </c>
       <c r="P21" s="1"/>
@@ -12995,15 +12998,15 @@
       <c r="J22" s="30">
         <v>4.4094344637268001</v>
       </c>
-      <c r="K22" s="30">
-        <f t="shared" si="1"/>
+      <c r="L22" s="30">
+        <f>(J22*2/3)+(M22/3)</f>
         <v>4.1107229120604369</v>
       </c>
-      <c r="L22" s="30">
+      <c r="M22" s="30">
         <f>H22</f>
         <v>3.5132998087277101</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>0</v>
       </c>
       <c r="P22" s="1"/>
@@ -13032,13 +13035,13 @@
       <c r="J23" s="30">
         <v>13.57977245</v>
       </c>
-      <c r="K23" s="30">
-        <v>0</v>
-      </c>
       <c r="L23" s="30">
         <v>0</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="30">
+        <v>0</v>
+      </c>
+      <c r="N23">
         <v>0</v>
       </c>
       <c r="P23" s="1"/>
@@ -13067,15 +13070,15 @@
       <c r="J24" s="30">
         <v>0.23</v>
       </c>
-      <c r="K24" s="30">
-        <f t="shared" si="1"/>
+      <c r="L24" s="30">
+        <f>(J24*2/3)+(M24/3)</f>
         <v>0.23116440009552636</v>
       </c>
-      <c r="L24" s="30">
+      <c r="M24" s="30">
         <f>H24</f>
         <v>0.23349320028657899</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>0</v>
       </c>
       <c r="P24" s="1"/>
@@ -13104,15 +13107,15 @@
       <c r="J25" s="30">
         <v>46.814427170000002</v>
       </c>
-      <c r="K25" s="30">
-        <f t="shared" si="1"/>
+      <c r="L25" s="30">
+        <f>(J25*2/3)+(M25/3)</f>
         <v>46.521563664810671</v>
       </c>
-      <c r="L25" s="30">
+      <c r="M25" s="30">
         <f>H25</f>
         <v>45.935836654432002</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>0</v>
       </c>
       <c r="P25" s="1"/>
@@ -13141,14 +13144,14 @@
       <c r="J26" s="30">
         <v>29.618106901468909</v>
       </c>
-      <c r="K26" s="30">
-        <f>J26*2/3+L26*1/3</f>
+      <c r="L26" s="30">
+        <f>J26*2/3+M26*1/3</f>
         <v>30.669454951005577</v>
       </c>
-      <c r="L26" s="30">
+      <c r="M26" s="30">
         <v>32.772151050078904</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>0</v>
       </c>
     </row>
@@ -13176,14 +13179,14 @@
       <c r="J27" s="30">
         <v>59.593058464401295</v>
       </c>
-      <c r="K27" s="30">
-        <f>J27*2/3+L27*1/3</f>
+      <c r="L27" s="30">
+        <f>J27*2/3+M27*1/3</f>
         <v>61.758486976267527</v>
       </c>
-      <c r="L27" s="30">
+      <c r="M27" s="30">
         <v>66.089343999999997</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>0</v>
       </c>
     </row>
@@ -13206,14 +13209,19 @@
         <v>5.6291760000000002</v>
       </c>
       <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="30">
-        <v>40.299999999999997</v>
+      <c r="J28" s="1">
+        <v>10.868399999999999</v>
+      </c>
+      <c r="K28" s="1">
+        <v>14.3748</v>
       </c>
       <c r="L28" s="30">
         <v>40.299999999999997</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="30">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="N28">
         <v>0</v>
       </c>
     </row>
@@ -13237,13 +13245,13 @@
       </c>
       <c r="I29" s="31"/>
       <c r="J29" s="31"/>
-      <c r="K29" s="31">
+      <c r="L29" s="31">
         <v>0.5</v>
       </c>
-      <c r="L29" s="30">
+      <c r="M29" s="30">
         <v>0.54</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>0</v>
       </c>
     </row>
@@ -13256,8 +13264,6 @@
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" t="s">

</xml_diff>

<commit_message>
Make LED scenario functional again
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E720B6E-E630-484F-B6DD-C97CE1C045D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A61235-A7D9-4CB3-B4EE-3E9A275FB570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -570,15 +570,6 @@
     <t>Development</t>
   </si>
   <si>
-    <t>RSDSH_Apt</t>
-  </si>
-  <si>
-    <t>RSDSH_Att</t>
-  </si>
-  <si>
-    <t>RSDSH_Det</t>
-  </si>
-  <si>
     <t>RSDSC_Apt</t>
   </si>
   <si>
@@ -781,6 +772,15 @@
   </si>
   <si>
     <t>Specify end-use demand projections (low energy demand variant)</t>
+  </si>
+  <si>
+    <t>RSDSH_Apt*</t>
+  </si>
+  <si>
+    <t>RSDSH_Att*</t>
+  </si>
+  <si>
+    <t>RSDSH_Det*</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -2429,10 +2429,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
@@ -2554,7 +2554,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
       <c r="B24" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
@@ -2584,7 +2584,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" s="42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B26" s="47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
@@ -2646,7 +2646,7 @@
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
       <c r="B27" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
@@ -2676,7 +2676,7 @@
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
       <c r="B28" s="42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B29" s="43">
         <v>1</v>
@@ -2737,10 +2737,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47"/>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="47"/>
@@ -2802,7 +2802,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="45"/>
       <c r="B32" s="46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="45"/>
@@ -6963,7 +6963,7 @@
         <v>2018</v>
       </c>
       <c r="I39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J39" s="21">
         <v>28.901664567933999</v>
@@ -7012,7 +7012,7 @@
         <v>2018</v>
       </c>
       <c r="I40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J40" s="21">
         <v>58.151541961987597</v>
@@ -7061,7 +7061,7 @@
         <v>2018</v>
       </c>
       <c r="I41" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J41" s="21">
         <v>5.6291760000000002</v>
@@ -7110,7 +7110,7 @@
         <v>2018</v>
       </c>
       <c r="I42" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J42" s="21">
         <v>0.48</v>
@@ -12232,7 +12232,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:AQ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -12250,7 +12250,7 @@
   <sheetData>
     <row r="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -12291,7 +12291,7 @@
         <v>2050</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
@@ -12319,7 +12319,7 @@
         <v>1.81463172003468</v>
       </c>
       <c r="L3" s="30">
-        <f>J3*2/3+M3/3</f>
+        <f t="shared" ref="L3:L16" si="0">J3*2/3+M3/3</f>
         <v>1.23293489482708</v>
       </c>
       <c r="M3" s="30">
@@ -12355,7 +12355,7 @@
         <v>22.997393933436499</v>
       </c>
       <c r="L4" s="30">
-        <f>J4*2/3+M4/3</f>
+        <f t="shared" si="0"/>
         <v>21.564038456241871</v>
       </c>
       <c r="M4" s="30">
@@ -12391,7 +12391,7 @@
         <v>1.3579701788487999</v>
       </c>
       <c r="L5" s="30">
-        <f>J5*2/3+M5/3</f>
+        <f t="shared" si="0"/>
         <v>1.8168912035156706</v>
       </c>
       <c r="M5" s="30">
@@ -12427,7 +12427,7 @@
         <v>5.7274313907438001</v>
       </c>
       <c r="L6" s="30">
-        <f>J6*2/3+M6/3</f>
+        <f t="shared" si="0"/>
         <v>5.2212845051183363</v>
       </c>
       <c r="M6" s="30">
@@ -12463,7 +12463,7 @@
         <v>1.1453307514123801</v>
       </c>
       <c r="L7" s="30">
-        <f>J7*2/3+M7/3</f>
+        <f t="shared" si="0"/>
         <v>1.1872938839576666</v>
       </c>
       <c r="M7" s="30">
@@ -12499,7 +12499,7 @@
         <v>10.4827865863979</v>
       </c>
       <c r="L8" s="30">
-        <f>J8*2/3+M8/3</f>
+        <f t="shared" si="0"/>
         <v>9.391476771293469</v>
       </c>
       <c r="M8" s="30">
@@ -12535,7 +12535,7 @@
         <v>1.05400776614231</v>
       </c>
       <c r="L9" s="30">
-        <f>J9*2/3+M9/3</f>
+        <f t="shared" si="0"/>
         <v>0.86541028956347699</v>
       </c>
       <c r="M9" s="30">
@@ -12571,7 +12571,7 @@
         <v>16.2067419529189</v>
       </c>
       <c r="L10" s="30">
-        <f>J10*2/3+M10/3</f>
+        <f t="shared" si="0"/>
         <v>13.7661776960718</v>
       </c>
       <c r="M10" s="30">
@@ -12607,7 +12607,7 @@
         <v>17.9214706310973</v>
       </c>
       <c r="L11" s="30">
-        <f>J11*2/3+M11/3</f>
+        <f t="shared" si="0"/>
         <v>15.932252704329224</v>
       </c>
       <c r="M11" s="30">
@@ -12643,7 +12643,7 @@
         <v>2.2861941894738802</v>
       </c>
       <c r="L12" s="30">
-        <f>J12*2/3+M12/3</f>
+        <f t="shared" si="0"/>
         <v>1.8333550602163233</v>
       </c>
       <c r="M12" s="30">
@@ -12679,7 +12679,7 @@
         <v>5.7966251432017799</v>
       </c>
       <c r="L13" s="30">
-        <f>J13*2/3+M13/3</f>
+        <f t="shared" si="0"/>
         <v>6.8655407588300337</v>
       </c>
       <c r="M13" s="30">
@@ -12715,7 +12715,7 @@
         <v>0.19444424313328701</v>
       </c>
       <c r="L14" s="30">
-        <f>J14*2/3+M14/3</f>
+        <f t="shared" si="0"/>
         <v>0.13734812058446252</v>
       </c>
       <c r="M14" s="30">
@@ -12751,7 +12751,7 @@
         <v>4.5897245674903298</v>
       </c>
       <c r="L15" s="30">
-        <f>J15*2/3+M15/3</f>
+        <f t="shared" si="0"/>
         <v>4.1809760165229068</v>
       </c>
       <c r="M15" s="30">
@@ -12787,7 +12787,7 @@
         <v>3.5251257971202601</v>
       </c>
       <c r="L16" s="30">
-        <f>J16*2/3+M16/3</f>
+        <f t="shared" si="0"/>
         <v>3.4314725583947805</v>
       </c>
       <c r="M16" s="30">
@@ -13129,10 +13129,10 @@
         <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G26" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H26" s="31">
         <f>VLOOKUP(F26,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
@@ -13164,10 +13164,10 @@
         <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H27" s="31">
         <f>VLOOKUP(F27,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
@@ -13199,10 +13199,10 @@
         <v>59</v>
       </c>
       <c r="F28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H28" s="31">
         <f>VLOOKUP(F28,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
@@ -13234,10 +13234,10 @@
         <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H29" s="31">
         <f>VLOOKUP(F29,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
@@ -13267,7 +13267,7 @@
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
@@ -13288,10 +13288,10 @@
         <v>3</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>4</v>
@@ -13399,7 +13399,7 @@
         <v>2050</v>
       </c>
       <c r="AQ33" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="3:43" x14ac:dyDescent="0.25">
@@ -13407,7 +13407,7 @@
         <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>52</v>
@@ -13524,7 +13524,7 @@
         <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>54</v>
@@ -13641,7 +13641,7 @@
         <v>59</v>
       </c>
       <c r="E36" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>56</v>
@@ -13806,8 +13806,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13820,7 +13820,7 @@
   <sheetData>
     <row r="4" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -13850,22 +13850,22 @@
         <v>4</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -13878,7 +13878,7 @@
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F7">
         <v>2020</v>
@@ -13890,18 +13890,18 @@
         <v>1.6534164675637491E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="J7" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="K7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F8">
         <v>2020</v>
@@ -13913,18 +13913,18 @@
         <v>2.9990596485367418E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="J8" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="K8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F9">
         <v>2020</v>
@@ -13936,21 +13936,21 @@
         <v>5.2849616307060754E-2</v>
       </c>
       <c r="I9" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="J9" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="K9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F10">
         <v>2020</v>
@@ -13962,21 +13962,21 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F11">
         <v>2020</v>
@@ -13988,21 +13988,21 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F12">
         <v>2020</v>
@@ -14014,18 +14014,18 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F13">
         <v>2020</v>
@@ -14037,18 +14037,18 @@
         <v>1.3128101846771158E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F14">
         <v>2020</v>
@@ -14060,18 +14060,18 @@
         <v>1.0994534987992988E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F15">
         <v>2020</v>
@@ -14083,18 +14083,18 @@
         <v>1.4648486376153701E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F16">
         <v>2020</v>
@@ -14106,18 +14106,18 @@
         <v>6.4458708104453747E-4</v>
       </c>
       <c r="I16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F17">
         <v>2020</v>
@@ -14129,18 +14129,18 @@
         <v>9.1487081392159866E-4</v>
       </c>
       <c r="I17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F18">
         <v>2020</v>
@@ -14152,18 +14152,18 @@
         <v>1.5069837916185766E-3</v>
       </c>
       <c r="I18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F19">
         <v>2020</v>
@@ -14175,18 +14175,18 @@
         <v>1.9923424990874787E-4</v>
       </c>
       <c r="I19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F20">
         <v>2020</v>
@@ -14198,18 +14198,18 @@
         <v>3.8001436556751221E-4</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F21">
         <v>2020</v>
@@ -14221,18 +14221,18 @@
         <v>4.7050395502371922E-4</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F22">
         <v>2050</v>
@@ -14244,18 +14244,18 @@
         <v>1.031688375401618E-2</v>
       </c>
       <c r="I22" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="J22" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="K22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F23">
         <v>2050</v>
@@ -14267,18 +14267,18 @@
         <v>1.031688375401618E-2</v>
       </c>
       <c r="I23" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="J23" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="K23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F24">
         <v>2050</v>
@@ -14290,21 +14290,21 @@
         <v>1.031688375401618E-2</v>
       </c>
       <c r="I24" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="J24" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="K24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F25">
         <v>2050</v>
@@ -14316,21 +14316,21 @@
         <v>1.8402644937451934E-4</v>
       </c>
       <c r="I25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F26">
         <v>2050</v>
@@ -14342,21 +14342,21 @@
         <v>1.8402644937451934E-4</v>
       </c>
       <c r="I26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F27">
         <v>2050</v>
@@ -14368,18 +14368,18 @@
         <v>1.8402644937451934E-4</v>
       </c>
       <c r="I27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F28">
         <v>2050</v>
@@ -14391,18 +14391,18 @@
         <v>5.4676481366779635E-3</v>
       </c>
       <c r="I28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F29">
         <v>2050</v>
@@ -14414,18 +14414,18 @@
         <v>5.4676481366779635E-3</v>
       </c>
       <c r="I29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K29" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F30">
         <v>2050</v>
@@ -14437,18 +14437,18 @@
         <v>5.4676481366779635E-3</v>
       </c>
       <c r="I30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F31">
         <v>2050</v>
@@ -14460,18 +14460,18 @@
         <v>9.2405926458938932E-4</v>
       </c>
       <c r="I31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F32">
         <v>2050</v>
@@ -14483,18 +14483,18 @@
         <v>9.2405926458938932E-4</v>
       </c>
       <c r="I32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F33">
         <v>2050</v>
@@ -14506,18 +14506,18 @@
         <v>9.2405926458938932E-4</v>
       </c>
       <c r="I33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K33" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F34">
         <v>2050</v>
@@ -14529,18 +14529,18 @@
         <v>1.4924076946288027E-3</v>
       </c>
       <c r="I34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F35">
         <v>2050</v>
@@ -14552,18 +14552,18 @@
         <v>1.4924076946288027E-3</v>
       </c>
       <c r="I35" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J35" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K35" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F36">
         <v>2050</v>
@@ -14575,18 +14575,18 @@
         <v>1.4924076946288027E-3</v>
       </c>
       <c r="I36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F37">
         <v>2050</v>
@@ -14598,18 +14598,18 @@
         <v>5.1051831876312761E-3</v>
       </c>
       <c r="I37" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="J37" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="K37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F38">
         <v>2050</v>
@@ -14621,18 +14621,18 @@
         <v>5.1051831876312761E-3</v>
       </c>
       <c r="I38" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="J38" t="s">
-        <v>135</v>
+        <v>203</v>
       </c>
       <c r="K38" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F39">
         <v>2050</v>
@@ -14644,18 +14644,18 @@
         <v>5.1051831876312761E-3</v>
       </c>
       <c r="I39" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="J39" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="K39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F40">
         <v>2050</v>
@@ -14667,18 +14667,18 @@
         <v>9.1063227794977141E-5</v>
       </c>
       <c r="I40" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J40" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F41">
         <v>2050</v>
@@ -14690,18 +14690,18 @@
         <v>9.1063227794977141E-5</v>
       </c>
       <c r="I41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F42">
         <v>2050</v>
@@ -14713,18 +14713,18 @@
         <v>9.1063227794977141E-5</v>
       </c>
       <c r="I42" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K42" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F43">
         <v>2050</v>
@@ -14736,18 +14736,18 @@
         <v>2.7055985129604311E-3</v>
       </c>
       <c r="I43" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J43" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F44">
         <v>2050</v>
@@ -14759,18 +14759,18 @@
         <v>2.7055985129604311E-3</v>
       </c>
       <c r="I44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K44" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F45">
         <v>2050</v>
@@ -14782,18 +14782,18 @@
         <v>2.7055985129604311E-3</v>
       </c>
       <c r="I45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K45" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F46">
         <v>2050</v>
@@ -14805,18 +14805,18 @@
         <v>4.5725937545048278E-4</v>
       </c>
       <c r="I46" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J46" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K46" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F47">
         <v>2050</v>
@@ -14828,18 +14828,18 @@
         <v>4.5725937545048278E-4</v>
       </c>
       <c r="I47" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J47" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F48">
         <v>2050</v>
@@ -14851,18 +14851,18 @@
         <v>4.5725937545048278E-4</v>
       </c>
       <c r="I48" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J48" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F49">
         <v>2050</v>
@@ -14874,18 +14874,18 @@
         <v>7.384996141634885E-4</v>
       </c>
       <c r="I49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F50">
         <v>2050</v>
@@ -14897,18 +14897,18 @@
         <v>7.384996141634885E-4</v>
       </c>
       <c r="I50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K50" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F51">
         <v>2050</v>
@@ -14920,13 +14920,13 @@
         <v>7.384996141634885E-4</v>
       </c>
       <c r="I51" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J51" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -14956,7 +14956,7 @@
   <sheetData>
     <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
@@ -14985,23 +14985,23 @@
         <v>4</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="N4" s="29"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -15013,7 +15013,7 @@
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F6">
         <v>2020</v>
@@ -15022,15 +15022,15 @@
         <v>0.29750119328038643</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F7">
         <v>2020</v>
@@ -15039,15 +15039,15 @@
         <v>7.8240205489280165E-2</v>
       </c>
       <c r="I7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F8">
         <v>2020</v>
@@ -15056,15 +15056,15 @@
         <v>9.9230285582155173E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F9">
         <v>2020</v>
@@ -15073,15 +15073,15 @@
         <v>0.1299964335480952</v>
       </c>
       <c r="I9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F10">
         <v>2020</v>
@@ -15090,15 +15090,15 @@
         <v>0.65611067742996398</v>
       </c>
       <c r="I10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F11">
         <v>2020</v>
@@ -15107,15 +15107,15 @@
         <v>3.4112422198348336</v>
       </c>
       <c r="I11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F12">
         <v>2020</v>
@@ -15124,15 +15124,15 @@
         <v>0.27048899641521007</v>
       </c>
       <c r="I12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F13">
         <v>2020</v>
@@ -15141,15 +15141,15 @@
         <v>0.14436837706846065</v>
       </c>
       <c r="I13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F14">
         <v>2020</v>
@@ -15158,15 +15158,15 @@
         <v>3.5851150535518087E-2</v>
       </c>
       <c r="I14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F15">
         <v>2020</v>
@@ -15175,15 +15175,15 @@
         <v>2.7014519280249845E-2</v>
       </c>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F16">
         <v>2020</v>
@@ -15192,15 +15192,15 @@
         <v>3.8223383014175182E-2</v>
       </c>
       <c r="I16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F17">
         <v>2020</v>
@@ -15209,15 +15209,15 @@
         <v>0.16206914757843674</v>
       </c>
       <c r="I17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F18">
         <v>2020</v>
@@ -15226,15 +15226,15 @@
         <v>0.84262783364201532</v>
       </c>
       <c r="I18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F19">
         <v>2020</v>
@@ -15243,15 +15243,15 @@
         <v>7.3395482092335179E-2</v>
       </c>
       <c r="I19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F20">
         <v>2050</v>
@@ -15260,15 +15260,15 @@
         <v>0.16362565630421255</v>
       </c>
       <c r="I20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F21">
         <v>2050</v>
@@ -15277,15 +15277,15 @@
         <v>4.3032113019104097E-2</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F22">
         <v>2050</v>
@@ -15294,15 +15294,15 @@
         <v>5.4576657070185351E-2</v>
       </c>
       <c r="I22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J22" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F23">
         <v>2050</v>
@@ -15311,15 +15311,15 @@
         <v>7.1498038451452361E-2</v>
       </c>
       <c r="I23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F24">
         <v>2050</v>
@@ -15328,15 +15328,15 @@
         <v>0.3608608725864802</v>
       </c>
       <c r="I24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F25">
         <v>2050</v>
@@ -15345,15 +15345,15 @@
         <v>1.8761832209091587</v>
       </c>
       <c r="I25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F26">
         <v>2050</v>
@@ -15362,15 +15362,15 @@
         <v>0.14876894802836554</v>
       </c>
       <c r="I26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F27">
         <v>2050</v>
@@ -15379,15 +15379,15 @@
         <v>7.9402607387653368E-2</v>
       </c>
       <c r="I27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F28">
         <v>2050</v>
@@ -15396,15 +15396,15 @@
         <v>1.9718132794534948E-2</v>
       </c>
       <c r="I28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F29">
         <v>2050</v>
@@ -15413,15 +15413,15 @@
         <v>1.4857985604137416E-2</v>
       </c>
       <c r="I29" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J29" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F30">
         <v>2050</v>
@@ -15430,15 +15430,15 @@
         <v>2.1022860657796353E-2</v>
       </c>
       <c r="I30" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J30" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F31">
         <v>2050</v>
@@ -15447,15 +15447,15 @@
         <v>8.9138031168140217E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F32">
         <v>2050</v>
@@ -15464,15 +15464,15 @@
         <v>0.46344530850310844</v>
       </c>
       <c r="I32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F33">
         <v>2050</v>
@@ -15481,10 +15481,10 @@
         <v>4.036751515078435E-2</v>
       </c>
       <c r="I33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specify demands and shares for IND for 2019-2021 based on EB
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A61235-A7D9-4CB3-B4EE-3E9A275FB570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CDC06E-A090-4400-940C-F27CE210A63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -5295,86 +5295,86 @@
         <v>42</v>
       </c>
       <c r="J10" s="20">
-        <v>7.7245727925227703</v>
+        <v>7.7105748259750104</v>
       </c>
       <c r="K10" s="21"/>
       <c r="L10" s="20">
-        <v>9.2353600579585193E-2</v>
+        <v>9.2186243413538399E-2</v>
       </c>
       <c r="M10" s="20">
-        <v>2.18565051154552</v>
+        <v>2.1816898183696698</v>
       </c>
       <c r="N10" s="20">
-        <v>0.36094016622216002</v>
+        <v>0.360286094015421</v>
       </c>
       <c r="O10" s="20">
-        <v>0.160971553655473</v>
+        <v>0.160679851514302</v>
       </c>
       <c r="P10" s="20">
-        <v>0.13739325701343899</v>
+        <v>0.13714428192223099</v>
       </c>
       <c r="Q10" s="20">
-        <v>6.6303111018221506E-2</v>
+        <v>6.6182960848759104E-2</v>
       </c>
       <c r="R10" s="20">
-        <v>0.20907225210952099</v>
+        <v>0.20869338502266699</v>
       </c>
       <c r="S10" s="20">
-        <v>0.31639527280693802</v>
+        <v>0.31582192194811698</v>
       </c>
       <c r="T10" s="20">
-        <v>0.126466294083908</v>
+        <v>0.12623712012159899</v>
       </c>
       <c r="U10" s="20">
-        <v>0.14400037102947</v>
+        <v>0.14373942295756001</v>
       </c>
       <c r="V10" s="20">
-        <v>0.24287511041201201</v>
+        <v>0.24243498799202201</v>
       </c>
       <c r="W10" s="20">
-        <v>0.23103810796296301</v>
+        <v>0.23061943578608199</v>
       </c>
       <c r="X10" s="20">
-        <v>0.19274182814699201</v>
+        <v>0.19239255398837901</v>
       </c>
       <c r="Y10" s="20">
-        <v>0.880626263602864</v>
+        <v>0.879030450176013</v>
       </c>
       <c r="Z10" s="20">
-        <v>0.239606430141375</v>
+        <v>0.23917223101039001</v>
       </c>
       <c r="AA10" s="20">
-        <v>0.31616005760135901</v>
+        <v>0.31558713298417801</v>
       </c>
       <c r="AB10" s="20">
-        <v>0.25882270135028701</v>
+        <v>0.25835367974707202</v>
       </c>
       <c r="AC10" s="20">
-        <v>0.18845766705778599</v>
+        <v>0.188116156376225</v>
       </c>
       <c r="AD10" s="20">
-        <v>0.418614934630201</v>
+        <v>0.41785634797321203</v>
       </c>
       <c r="AE10" s="20">
-        <v>5.1980938259190403E-2</v>
+        <v>5.1886741796237999E-2</v>
       </c>
       <c r="AF10" s="20">
-        <v>0.21170504023817699</v>
+        <v>0.21132140218454701</v>
       </c>
       <c r="AG10" s="20">
-        <v>0.104701587785582</v>
+        <v>0.104511854403208</v>
       </c>
       <c r="AH10" s="20">
-        <v>0.106309162052679</v>
+        <v>0.106116515529162</v>
       </c>
       <c r="AI10" s="20">
-        <v>0.12357071379453501</v>
+        <v>0.123346787013801</v>
       </c>
       <c r="AJ10" s="20">
-        <v>0.25823709659708599</v>
+        <v>0.257769136188576</v>
       </c>
       <c r="AK10" s="20">
-        <v>9.95787628254481E-2</v>
+        <v>9.9398312692044299E-2</v>
       </c>
     </row>
     <row r="11" spans="3:37" x14ac:dyDescent="0.25">
@@ -5493,86 +5493,86 @@
         <v>46</v>
       </c>
       <c r="J12" s="20">
-        <v>21.784659175997099</v>
+        <v>20.831454920682301</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12" s="20">
-        <v>0.26045346019004401</v>
+        <v>0.24905712185126699</v>
       </c>
       <c r="M12" s="20">
-        <v>6.1639203553045503</v>
+        <v>5.8942133534813896</v>
       </c>
       <c r="N12" s="20">
-        <v>1.0179149987024101</v>
+        <v>0.97337535727524804</v>
       </c>
       <c r="O12" s="20">
-        <v>0.45396820349853301</v>
+        <v>0.434104481057138</v>
       </c>
       <c r="P12" s="20">
-        <v>0.387473243829765</v>
+        <v>0.37051905869171597</v>
       </c>
       <c r="Q12" s="20">
-        <v>0.18698647998221901</v>
+        <v>0.17880474498396101</v>
       </c>
       <c r="R12" s="20">
-        <v>0.58962066611279595</v>
+        <v>0.56382136746783496</v>
       </c>
       <c r="S12" s="20">
-        <v>0.89229053413382597</v>
+        <v>0.85324768626358805</v>
       </c>
       <c r="T12" s="20">
-        <v>0.35665727903246103</v>
+        <v>0.34105146976474798</v>
       </c>
       <c r="U12" s="20">
-        <v>0.40610647195022498</v>
+        <v>0.38833697580863102</v>
       </c>
       <c r="V12" s="20">
-        <v>0.68495069497951599</v>
+        <v>0.654980158747549</v>
       </c>
       <c r="W12" s="20">
-        <v>0.65156825805464502</v>
+        <v>0.62305839562402099</v>
       </c>
       <c r="X12" s="20">
-        <v>0.54356598713202597</v>
+        <v>0.51978184583366205</v>
       </c>
       <c r="Y12" s="20">
-        <v>2.4835215524915499</v>
+        <v>2.3748531866991098</v>
       </c>
       <c r="Z12" s="20">
-        <v>0.67573243947675998</v>
+        <v>0.64616525499341604</v>
       </c>
       <c r="AA12" s="20">
-        <v>0.89162718572295796</v>
+        <v>0.85261336316465597</v>
       </c>
       <c r="AB12" s="20">
-        <v>0.72992571723638999</v>
+        <v>0.69798726485518303</v>
       </c>
       <c r="AC12" s="20">
-        <v>0.53148389642096905</v>
+        <v>0.50822841614896397</v>
       </c>
       <c r="AD12" s="20">
-        <v>1.1805680290473299</v>
+        <v>1.1289113811335301</v>
       </c>
       <c r="AE12" s="20">
-        <v>0.146595423985277</v>
+        <v>0.140181030222055</v>
       </c>
       <c r="AF12" s="20">
-        <v>0.59704559349789399</v>
+        <v>0.57092141153381903</v>
       </c>
       <c r="AG12" s="20">
-        <v>0.29527696435231898</v>
+        <v>0.28235689722420099</v>
       </c>
       <c r="AH12" s="20">
-        <v>0.29981060762935702</v>
+        <v>0.28669216750725102</v>
       </c>
       <c r="AI12" s="20">
-        <v>0.34849123135384003</v>
+        <v>0.33324273368478402</v>
       </c>
       <c r="AJ12" s="20">
-        <v>0.72827420843415902</v>
+        <v>0.69640801907094396</v>
       </c>
       <c r="AK12" s="20">
-        <v>0.28082969344526898</v>
+        <v>0.268541777593654</v>
       </c>
     </row>
     <row r="13" spans="3:37" x14ac:dyDescent="0.25">
@@ -5691,14 +5691,14 @@
         <v>50</v>
       </c>
       <c r="J14" s="20">
-        <v>45.935836654432002</v>
+        <v>45.9683637522608</v>
       </c>
       <c r="K14" s="21"/>
       <c r="L14" s="20">
         <v>0</v>
       </c>
       <c r="M14" s="20">
-        <v>40.411547456014503</v>
+        <v>40.4401628128524</v>
       </c>
       <c r="N14" s="20">
         <v>0</v>
@@ -5731,13 +5731,13 @@
         <v>0</v>
       </c>
       <c r="X14" s="20">
-        <v>2.3928132767411898</v>
+        <v>2.39450762427477</v>
       </c>
       <c r="Y14" s="20">
-        <v>2.2124403851853902</v>
+        <v>2.2140070109418901</v>
       </c>
       <c r="Z14" s="20">
-        <v>0.24110252653151401</v>
+        <v>0.24127325087308299</v>
       </c>
       <c r="AA14" s="20">
         <v>0</v>
@@ -5755,7 +5755,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="20">
-        <v>0.68832808501139198</v>
+        <v>0.68881548910784596</v>
       </c>
       <c r="AG14" s="20">
         <v>0</v>
@@ -6280,10 +6280,10 @@
         <v>6</v>
       </c>
       <c r="J25" s="20">
-        <v>2.0712927345907701</v>
+        <v>1.8983540603270901</v>
       </c>
       <c r="K25" s="20">
-        <v>2.0712927345907701</v>
+        <v>1.8983540603270901</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
@@ -6329,10 +6329,10 @@
         <v>8</v>
       </c>
       <c r="J26" s="20">
-        <v>22.2490403410117</v>
+        <v>20.1128233846323</v>
       </c>
       <c r="K26" s="20">
-        <v>22.2490403410117</v>
+        <v>20.1128233846323</v>
       </c>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -6378,10 +6378,10 @@
         <v>10</v>
       </c>
       <c r="J27" s="20">
-        <v>1.2014578872914701</v>
+        <v>0.42769784899188301</v>
       </c>
       <c r="K27" s="20">
-        <v>1.2014578872914701</v>
+        <v>0.42769784899188301</v>
       </c>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
@@ -6427,10 +6427,10 @@
         <v>12</v>
       </c>
       <c r="J28" s="20">
-        <v>6.6890404714869804</v>
+        <v>6.9295287156334302</v>
       </c>
       <c r="K28" s="20">
-        <v>6.6890404714869804</v>
+        <v>6.9295287156334302</v>
       </c>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
@@ -6476,10 +6476,10 @@
         <v>14</v>
       </c>
       <c r="J29" s="20">
-        <v>0.67287296253748397</v>
+        <v>1.09140526535876</v>
       </c>
       <c r="K29" s="20">
-        <v>0.67287296253748397</v>
+        <v>1.09140526535876</v>
       </c>
       <c r="L29" s="21"/>
       <c r="M29" s="21"/>
@@ -6525,10 +6525,10 @@
         <v>16</v>
       </c>
       <c r="J30" s="20">
-        <v>10.5976971594968</v>
+        <v>9.5100483128062994</v>
       </c>
       <c r="K30" s="20">
-        <v>10.5976971594968</v>
+        <v>9.5100483128062994</v>
       </c>
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
@@ -6574,10 +6574,10 @@
         <v>18</v>
       </c>
       <c r="J31" s="20">
-        <v>1.14056826967015</v>
+        <v>1.9556249526505201</v>
       </c>
       <c r="K31" s="20">
-        <v>1.14056826967015</v>
+        <v>1.9556249526505201</v>
       </c>
       <c r="L31" s="21"/>
       <c r="M31" s="21"/>
@@ -6623,10 +6623,10 @@
         <v>20</v>
       </c>
       <c r="J32" s="20">
-        <v>17.770098364755199</v>
+        <v>19.482476804508799</v>
       </c>
       <c r="K32" s="20">
-        <v>17.770098364755199</v>
+        <v>19.482476804508799</v>
       </c>
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
@@ -6672,10 +6672,10 @@
         <v>22</v>
       </c>
       <c r="J33" s="20">
-        <v>19.5397050142764</v>
+        <v>20.3153817696899</v>
       </c>
       <c r="K33" s="20">
-        <v>19.5397050142764</v>
+        <v>20.3153817696899</v>
       </c>
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
@@ -6721,10 +6721,10 @@
         <v>24</v>
       </c>
       <c r="J34" s="20">
-        <v>1.28965569884044</v>
+        <v>1.4729468330623701</v>
       </c>
       <c r="K34" s="20">
-        <v>1.28965569884044</v>
+        <v>1.4729468330623701</v>
       </c>
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
@@ -6770,10 +6770,10 @@
         <v>26</v>
       </c>
       <c r="J35" s="20">
-        <v>4.2689583715443504</v>
+        <v>4.65085642477431</v>
       </c>
       <c r="K35" s="20">
-        <v>4.2689583715443504</v>
+        <v>4.65085642477431</v>
       </c>
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
@@ -6819,10 +6819,10 @@
         <v>28</v>
       </c>
       <c r="J36" s="20">
-        <v>0.16518244671693</v>
+        <v>0.1947788154134</v>
       </c>
       <c r="K36" s="20">
-        <v>0.16518244671693</v>
+        <v>0.1947788154134</v>
       </c>
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
@@ -6868,10 +6868,10 @@
         <v>30</v>
       </c>
       <c r="J37" s="20">
-        <v>4.2546573385120396</v>
+        <v>4.6984287524850101</v>
       </c>
       <c r="K37" s="20">
-        <v>4.2546573385120396</v>
+        <v>4.6984287524850101</v>
       </c>
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
@@ -6917,10 +6917,10 @@
         <v>32</v>
       </c>
       <c r="J38" s="20">
-        <v>4.0239683065477196</v>
+        <v>1.9571195447376</v>
       </c>
       <c r="K38" s="20">
-        <v>4.0239683065477196</v>
+        <v>1.9571195447376</v>
       </c>
       <c r="L38" s="21"/>
       <c r="M38" s="21"/>
@@ -9160,15 +9160,15 @@
       </c>
       <c r="G20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13064779508364899</v>
+        <v>0.13064779508364888</v>
       </c>
       <c r="H20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.0919251481787136</v>
+        <v>3.091925148178714</v>
       </c>
       <c r="I20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.51060312297639665</v>
+        <v>0.51060312297639654</v>
       </c>
       <c r="J20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -9176,91 +9176,91 @@
       </c>
       <c r="K20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1943630348521006</v>
+        <v>0.19436303485210071</v>
       </c>
       <c r="L20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.3795533767547012E-2</v>
+        <v>9.379553376754686E-2</v>
       </c>
       <c r="M20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29576354987636128</v>
+        <v>0.29576354987636116</v>
       </c>
       <c r="N20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4475877985016371</v>
+        <v>0.44758779850163755</v>
       </c>
       <c r="O20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1789052334805798</v>
+        <v>0.17890523348057963</v>
       </c>
       <c r="P20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.20370977252820086</v>
+        <v>0.20370977252820055</v>
       </c>
       <c r="Q20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3435826806631439</v>
+        <v>0.34358268066314335</v>
       </c>
       <c r="R20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.32683749411207558</v>
+        <v>0.32683749411207597</v>
       </c>
       <c r="S20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.27266175557601846</v>
+        <v>0.2726617555760189</v>
       </c>
       <c r="T20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.2457757890372787</v>
+        <v>1.245775789037278</v>
       </c>
       <c r="U20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33895865011628784</v>
+        <v>0.33895865011628845</v>
       </c>
       <c r="V20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.44725505188660325</v>
+        <v>0.44725505188660303</v>
       </c>
       <c r="W20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3661429011624644</v>
+        <v>0.36614290116246478</v>
       </c>
       <c r="X20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26660117757391238</v>
+        <v>0.26660117757391266</v>
       </c>
       <c r="Y20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.5921925929827917</v>
+        <v>0.59219259298279137</v>
       </c>
       <c r="Z20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>7.3534707118324452E-2</v>
+        <v>7.3534707118324327E-2</v>
       </c>
       <c r="AA20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29948801716050255</v>
+        <v>0.2994880171605025</v>
       </c>
       <c r="AB20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14811584497082575</v>
+        <v>0.14811584497082581</v>
       </c>
       <c r="AC20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15038999597426655</v>
+        <v>0.15038999597426658</v>
       </c>
       <c r="AD20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17480900790929571</v>
+        <v>0.17480900790929638</v>
       </c>
       <c r="AE20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36531447683124091</v>
+        <v>0.36531447683124146</v>
       </c>
       <c r="AF20" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E20,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F20,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E20,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.14086885317580392</v>
+        <v>0.14086885317580389</v>
       </c>
     </row>
     <row r="21" spans="4:32" x14ac:dyDescent="0.25">
@@ -9275,15 +9275,15 @@
       </c>
       <c r="G21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.11877072280331726</v>
+        <v>0.11877072280331716</v>
       </c>
       <c r="H21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.8108410437988307</v>
+        <v>2.8108410437988312</v>
       </c>
       <c r="I21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.46418465725126973</v>
+        <v>0.46418465725126962</v>
       </c>
       <c r="J21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -9291,91 +9291,91 @@
       </c>
       <c r="K21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17669366804736417</v>
+        <v>0.17669366804736431</v>
       </c>
       <c r="L21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>8.5268667061406372E-2</v>
+        <v>8.5268667061406234E-2</v>
       </c>
       <c r="M21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.26887595443305573</v>
+        <v>0.26887595443305556</v>
       </c>
       <c r="N21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40689799863785192</v>
+        <v>0.40689799863785231</v>
       </c>
       <c r="O21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16264112134598166</v>
+        <v>0.16264112134598149</v>
       </c>
       <c r="P21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18519070229836443</v>
+        <v>0.18519070229836415</v>
       </c>
       <c r="Q21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.31234789151194903</v>
+        <v>0.31234789151194853</v>
       </c>
       <c r="R21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.29712499464734149</v>
+        <v>0.29712499464734182</v>
       </c>
       <c r="S21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2478743232509259</v>
+        <v>0.24787432325092632</v>
       </c>
       <c r="T21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.1325234445793442</v>
+        <v>1.1325234445793435</v>
       </c>
       <c r="U21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.30814422737844349</v>
+        <v>0.30814422737844405</v>
       </c>
       <c r="V21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4065955017150939</v>
+        <v>0.40659550171509368</v>
       </c>
       <c r="W21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33285718287496763</v>
+        <v>0.33285718287496796</v>
       </c>
       <c r="X21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.2423647068853749</v>
+        <v>0.24236470688537518</v>
       </c>
       <c r="Y21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.53835690271162884</v>
+        <v>0.53835690271162862</v>
       </c>
       <c r="Z21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>6.6849733743931328E-2</v>
+        <v>6.6849733743931203E-2</v>
       </c>
       <c r="AA21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.27226183378227509</v>
+        <v>0.27226183378227498</v>
       </c>
       <c r="AB21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13465076815529611</v>
+        <v>0.13465076815529617</v>
       </c>
       <c r="AC21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.13671817815842413</v>
+        <v>0.13671817815842419</v>
       </c>
       <c r="AD21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.15891727991754154</v>
+        <v>0.15891727991754215</v>
       </c>
       <c r="AE21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33210406984658275</v>
+        <v>0.33210406984658314</v>
       </c>
       <c r="AF21" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E21,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F21,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E21,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.12806259379618537</v>
+        <v>0.12806259379618534</v>
       </c>
     </row>
     <row r="22" spans="4:32" x14ac:dyDescent="0.25">
@@ -10082,107 +10082,107 @@
       </c>
       <c r="G28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.1629624043332934</v>
+        <v>0.16296240433329362</v>
       </c>
       <c r="H28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.8566862597502731</v>
+        <v>3.8566862597502802</v>
       </c>
       <c r="I28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.63689641701986843</v>
+        <v>0.63689641701986988</v>
       </c>
       <c r="J28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28404210824846116</v>
+        <v>0.28404210824846177</v>
       </c>
       <c r="K28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24243706105207907</v>
+        <v>0.24243706105207927</v>
       </c>
       <c r="L28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.11699505291074819</v>
+        <v>0.11699505291074846</v>
       </c>
       <c r="M28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.36891812197168955</v>
+        <v>0.36891812197169027</v>
       </c>
       <c r="N28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.55829479362718504</v>
+        <v>0.55829479362718626</v>
       </c>
       <c r="O28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.22315590536478461</v>
+        <v>0.22315590536478441</v>
       </c>
       <c r="P28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25409563396097901</v>
+        <v>0.25409563396097939</v>
       </c>
       <c r="Q28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42856490377273548</v>
+        <v>0.42856490377273632</v>
       </c>
       <c r="R28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4076779392462821</v>
+        <v>0.40767793924628298</v>
       </c>
       <c r="S28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.34010229740161857</v>
+        <v>0.34010229740161924</v>
       </c>
       <c r="T28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5539077235229115</v>
+        <v>1.5539077235229135</v>
       </c>
       <c r="U28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42279715901176512</v>
+        <v>0.42279715901176562</v>
       </c>
       <c r="V28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.5578797449967432</v>
+        <v>0.55787974499674464</v>
       </c>
       <c r="W28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45670520091670769</v>
+        <v>0.45670520091670846</v>
       </c>
       <c r="X28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33254268751887739</v>
+        <v>0.3325426875188775</v>
       </c>
       <c r="Y28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.738666341204264</v>
+        <v>0.73866634120426122</v>
       </c>
       <c r="Z28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.1722884923348305E-2</v>
+        <v>9.172288492334861E-2</v>
       </c>
       <c r="AA28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.37356380422829233</v>
+        <v>0.37356380422829349</v>
       </c>
       <c r="AB28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18475102622932804</v>
+        <v>0.1847510262293284</v>
       </c>
       <c r="AC28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18758766893807341</v>
+        <v>0.1875876689380738</v>
       </c>
       <c r="AD28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.21804651360382518</v>
+        <v>0.21804651360382526</v>
       </c>
       <c r="AE28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45567187294712425</v>
+        <v>0.45567187294712524</v>
       </c>
       <c r="AF28" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E28,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F28,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E28,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17571155329873456</v>
+        <v>0.17571155329873506</v>
       </c>
     </row>
     <row r="29" spans="4:32" x14ac:dyDescent="0.25">
@@ -10198,107 +10198,107 @@
       </c>
       <c r="G29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.16235731275947515</v>
+        <v>0.16235731275947538</v>
       </c>
       <c r="H29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>3.8423660957334085</v>
+        <v>3.8423660957334147</v>
       </c>
       <c r="I29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.63453157307374231</v>
+        <v>0.63453157307374375</v>
       </c>
       <c r="J29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.28298743869437681</v>
+        <v>0.28298743869437742</v>
       </c>
       <c r="K29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24153687414440531</v>
+        <v>0.2415368741444055</v>
       </c>
       <c r="L29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.11656064154461539</v>
+        <v>0.11656064154461564</v>
       </c>
       <c r="M29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3675483014419349</v>
+        <v>0.36754830144193562</v>
       </c>
       <c r="N29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.55622180337699523</v>
+        <v>0.55622180337699645</v>
       </c>
       <c r="O29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.22232731082767995</v>
+        <v>0.22232731082767976</v>
       </c>
       <c r="P29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.25315215790168288</v>
+        <v>0.25315215790168333</v>
       </c>
       <c r="Q29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.42697361028901426</v>
+        <v>0.42697361028901515</v>
       </c>
       <c r="R29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.40616420062123709</v>
+        <v>0.40616420062123793</v>
       </c>
       <c r="S29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.3388394721798389</v>
+        <v>0.33883947217983951</v>
       </c>
       <c r="T29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>1.5481379481330504</v>
+        <v>1.5481379481330526</v>
       </c>
       <c r="U29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.4212272815949526</v>
+        <v>0.42122728159495315</v>
       </c>
       <c r="V29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.55580829585310521</v>
+        <v>0.55580829585310654</v>
       </c>
       <c r="W29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45500942040877851</v>
+        <v>0.45500942040877934</v>
       </c>
       <c r="X29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.33130793169298151</v>
+        <v>0.33130793169298156</v>
       </c>
       <c r="Y29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.73592361793165129</v>
+        <v>0.73592361793164862</v>
       </c>
       <c r="Z29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>9.1382311003734881E-2</v>
+        <v>9.1382311003735187E-2</v>
       </c>
       <c r="AA29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.37217673393347922</v>
+        <v>0.37217673393348039</v>
       </c>
       <c r="AB29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18406503187570397</v>
+        <v>0.18406503187570436</v>
       </c>
       <c r="AC29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.18689114191829229</v>
+        <v>0.1868911419182927</v>
       </c>
       <c r="AD29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.21723689061978846</v>
+        <v>0.21723689061978854</v>
       </c>
       <c r="AE29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.45397992926309294</v>
+        <v>0.45397992926309383</v>
       </c>
       <c r="AF29" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E29,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F29,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E29,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.17505912318297531</v>
+        <v>0.17505912318297578</v>
       </c>
     </row>
     <row r="30" spans="4:32" x14ac:dyDescent="0.25">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="H36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>40.559731289160872</v>
+        <v>40.559731289160858</v>
       </c>
       <c r="I36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11055,15 +11055,15 @@
       </c>
       <c r="S36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.401587408534509</v>
+        <v>2.4015874085345037</v>
       </c>
       <c r="T36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.2205531132921634</v>
+        <v>2.2205531132921612</v>
       </c>
       <c r="U36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24198661780769198</v>
+        <v>0.24198661780769171</v>
       </c>
       <c r="V36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11087,7 +11087,7 @@
       </c>
       <c r="AA36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.6908520936307182</v>
+        <v>0.69085209363071676</v>
       </c>
       <c r="AB36" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E36,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F36,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E36,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="H37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>41.184477806263274</v>
+        <v>41.184477806263253</v>
       </c>
       <c r="I37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11171,15 +11171,15 @@
       </c>
       <c r="S37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.4385793540260186</v>
+        <v>2.4385793540260137</v>
       </c>
       <c r="T37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.2547565653239303</v>
+        <v>2.2547565653239281</v>
       </c>
       <c r="U37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24571396736982151</v>
+        <v>0.24571396736982123</v>
       </c>
       <c r="V37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11203,7 +11203,7 @@
       </c>
       <c r="AA37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.70149337318584271</v>
+        <v>0.70149337318584126</v>
       </c>
       <c r="AB37" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E37,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F37,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E37,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11243,7 +11243,7 @@
       </c>
       <c r="H38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>40.92683435618035</v>
+        <v>40.936372808459637</v>
       </c>
       <c r="I38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11287,15 +11287,15 @@
       </c>
       <c r="S38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.4233239949310756</v>
+        <v>2.4238887774422655</v>
       </c>
       <c r="T38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.2406511719444171</v>
+        <v>2.2411733805299154</v>
       </c>
       <c r="U38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24417682042371905</v>
+        <v>0.24423372853757513</v>
       </c>
       <c r="V38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11319,7 +11319,7 @@
       </c>
       <c r="AA38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.69710494379435917</v>
+        <v>0.69726741182650953</v>
       </c>
       <c r="AB38" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E38,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F38,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E38,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11359,7 +11359,7 @@
       </c>
       <c r="H39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>40.411547456014503</v>
+        <v>40.4401628128524</v>
       </c>
       <c r="I39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11403,15 +11403,15 @@
       </c>
       <c r="S39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.3928132767411898</v>
+        <v>2.39450762427477</v>
       </c>
       <c r="T39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>2.2124403851853902</v>
+        <v>2.2140070109418901</v>
       </c>
       <c r="U39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.24110252653151398</v>
+        <v>0.24127325087308299</v>
       </c>
       <c r="V39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -11435,7 +11435,7 @@
       </c>
       <c r="AA39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
-        <v>0.68832808501139198</v>
+        <v>0.68881548910784596</v>
       </c>
       <c r="AB39" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E39,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F39,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$H$2:$CO$25,MATCH($E39,DEMANDS!$F$2:$F$25,0),FALSE)</f>
@@ -12232,8 +12232,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:AQ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12310,17 +12310,20 @@
       </c>
       <c r="H3" s="31">
         <f>VLOOKUP(F3,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>2.0712927345907701</v>
+        <v>1.8983540603270901</v>
       </c>
       <c r="I3" s="30">
-        <v>2.0621875423309999</v>
+        <v>2.9169885814082672</v>
       </c>
       <c r="J3" s="30">
-        <v>1.81463172003468</v>
+        <v>2.9233084199020065</v>
+      </c>
+      <c r="K3" s="30">
+        <v>2.9160581250770159</v>
       </c>
       <c r="L3" s="30">
         <f t="shared" ref="L3:L16" si="0">J3*2/3+M3/3</f>
-        <v>1.23293489482708</v>
+        <v>1.972052694738631</v>
       </c>
       <c r="M3" s="30">
         <v>6.9541244411880462E-2</v>
@@ -12346,17 +12349,20 @@
       </c>
       <c r="H4" s="31">
         <f>VLOOKUP(F4,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>22.2490403410117</v>
+        <v>20.1128233846323</v>
       </c>
       <c r="I4" s="30">
-        <v>21.6662880683004</v>
+        <v>20.829707214475608</v>
       </c>
       <c r="J4" s="30">
-        <v>22.997393933436499</v>
+        <v>21.483394248547164</v>
+      </c>
+      <c r="K4" s="30">
+        <v>20.570384916097975</v>
       </c>
       <c r="L4" s="30">
         <f t="shared" si="0"/>
-        <v>21.564038456241871</v>
+        <v>20.554705332982316</v>
       </c>
       <c r="M4" s="30">
         <v>18.697327501852616</v>
@@ -12382,17 +12388,20 @@
       </c>
       <c r="H5" s="31">
         <f>VLOOKUP(F5,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>1.2014578872914701</v>
+        <v>0.42769784899188301</v>
       </c>
       <c r="I5" s="30">
-        <v>1.2266704416391101</v>
+        <v>0.74181807651109255</v>
       </c>
       <c r="J5" s="30">
-        <v>1.3579701788487999</v>
+        <v>0.7440570217426532</v>
+      </c>
+      <c r="K5" s="30">
+        <v>0.73064036372909791</v>
       </c>
       <c r="L5" s="30">
         <f t="shared" si="0"/>
-        <v>1.8168912035156706</v>
+        <v>1.407615765444906</v>
       </c>
       <c r="M5" s="30">
         <v>2.7347332528494115</v>
@@ -12418,17 +12427,20 @@
       </c>
       <c r="H6" s="31">
         <f>VLOOKUP(F6,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>6.6890404714869804</v>
+        <v>6.9295287156334302</v>
       </c>
       <c r="I6" s="30">
-        <v>6.45095434431237</v>
+        <v>6.5639975672352229</v>
       </c>
       <c r="J6" s="30">
-        <v>5.7274313907438001</v>
+        <v>5.780638065059601</v>
+      </c>
+      <c r="K6" s="30">
+        <v>6.5949264310858817</v>
       </c>
       <c r="L6" s="30">
         <f t="shared" si="0"/>
-        <v>5.2212845051183363</v>
+        <v>5.2567556213288702</v>
       </c>
       <c r="M6" s="30">
         <v>4.2089907338674086</v>
@@ -12454,17 +12466,20 @@
       </c>
       <c r="H7" s="31">
         <f>VLOOKUP(F7,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>0.67287296253748397</v>
+        <v>1.09140526535876</v>
       </c>
       <c r="I7" s="30">
-        <v>0.68901566323930896</v>
+        <v>0.5707726774555677</v>
       </c>
       <c r="J7" s="30">
-        <v>1.1453307514123801</v>
+        <v>0.56119057639608538</v>
+      </c>
+      <c r="K7" s="30">
+        <v>0.55161044480654198</v>
       </c>
       <c r="L7" s="30">
         <f t="shared" si="0"/>
-        <v>1.1872938839576666</v>
+        <v>0.7978671006134701</v>
       </c>
       <c r="M7" s="30">
         <v>1.2712201490482398</v>
@@ -12490,17 +12505,20 @@
       </c>
       <c r="H8" s="31">
         <f>VLOOKUP(F8,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>10.5976971594968</v>
+        <v>9.5100483128062994</v>
       </c>
       <c r="I8" s="30">
-        <v>10.425059758064601</v>
+        <v>9.7037603897089575</v>
       </c>
       <c r="J8" s="30">
-        <v>10.4827865863979</v>
+        <v>9.435975307949354</v>
+      </c>
+      <c r="K8" s="30">
+        <v>9.2516395819175106</v>
       </c>
       <c r="L8" s="30">
         <f t="shared" si="0"/>
-        <v>9.391476771293469</v>
+        <v>8.6936025856611057</v>
       </c>
       <c r="M8" s="30">
         <v>7.2088571410846098</v>
@@ -12526,17 +12544,20 @@
       </c>
       <c r="H9" s="31">
         <f>VLOOKUP(F9,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>1.14056826967015</v>
+        <v>1.9556249526505201</v>
       </c>
       <c r="I9" s="30">
-        <v>1.17</v>
+        <v>1.5498072549825794</v>
       </c>
       <c r="J9" s="30">
-        <v>1.05400776614231</v>
+        <v>1.5053268122598555</v>
+      </c>
+      <c r="K9" s="30">
+        <v>1.4894503267095116</v>
       </c>
       <c r="L9" s="30">
         <f t="shared" si="0"/>
-        <v>0.86541028956347699</v>
+        <v>1.1662896536418408</v>
       </c>
       <c r="M9" s="30">
         <v>0.48821533640581133</v>
@@ -12562,17 +12583,20 @@
       </c>
       <c r="H10" s="31">
         <f>VLOOKUP(F10,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>17.770098364755199</v>
+        <v>19.482476804508799</v>
       </c>
       <c r="I10" s="30">
-        <v>17.352426464494599</v>
+        <v>17.613308735917627</v>
       </c>
       <c r="J10" s="30">
-        <v>16.2067419529189</v>
+        <v>17.067480468046199</v>
+      </c>
+      <c r="K10" s="30">
+        <v>18.473544022536192</v>
       </c>
       <c r="L10" s="30">
         <f t="shared" si="0"/>
-        <v>13.7661776960718</v>
+        <v>14.340003372823332</v>
       </c>
       <c r="M10" s="30">
         <v>8.8850491823775997</v>
@@ -12598,17 +12622,20 @@
       </c>
       <c r="H11" s="31">
         <f>VLOOKUP(F11,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>19.5397050142764</v>
+        <v>20.3153817696899</v>
       </c>
       <c r="I11" s="30">
-        <v>20.047656182086499</v>
+        <v>20.746846228178715</v>
       </c>
       <c r="J11" s="30">
-        <v>17.9214706310973</v>
+        <v>18.66727780331064</v>
+      </c>
+      <c r="K11" s="30">
+        <v>19.411458005544933</v>
       </c>
       <c r="L11" s="30">
         <f t="shared" si="0"/>
-        <v>15.932252704329224</v>
+        <v>16.429457485804782</v>
       </c>
       <c r="M11" s="30">
         <v>11.953816850793071</v>
@@ -12634,17 +12661,20 @@
       </c>
       <c r="H12" s="31">
         <f>VLOOKUP(F12,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>1.28965569884044</v>
+        <v>1.4729468330623701</v>
       </c>
       <c r="I12" s="30">
-        <v>1.3174050900000001</v>
+        <v>1.4943226387301358</v>
       </c>
       <c r="J12" s="30">
-        <v>2.2861941894738802</v>
+        <v>1.4634791461847667</v>
+      </c>
+      <c r="K12" s="30">
+        <v>1.4446377495642824</v>
       </c>
       <c r="L12" s="30">
         <f t="shared" si="0"/>
-        <v>1.8333550602163233</v>
+        <v>1.2848783646902477</v>
       </c>
       <c r="M12" s="30">
         <v>0.92767680170120992</v>
@@ -12670,17 +12700,20 @@
       </c>
       <c r="H13" s="31">
         <f>VLOOKUP(F13,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>4.2689583715443504</v>
+        <v>4.65085642477431</v>
       </c>
       <c r="I13" s="30">
-        <v>5.7587113786598101</v>
+        <v>5.007589393109674</v>
       </c>
       <c r="J13" s="30">
-        <v>5.7966251432017799</v>
+        <v>4.7554316434518897</v>
+      </c>
+      <c r="K13" s="30">
+        <v>4.7269471440454405</v>
       </c>
       <c r="L13" s="30">
         <f t="shared" si="0"/>
-        <v>6.8655407588300337</v>
+        <v>6.1714117589967739</v>
       </c>
       <c r="M13" s="30">
         <v>9.0033719900865421</v>
@@ -12706,17 +12739,20 @@
       </c>
       <c r="H14" s="31">
         <f>VLOOKUP(F14,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>0.16518244671693</v>
+        <v>0.1947788154134</v>
       </c>
       <c r="I14" s="30">
-        <v>0.19765643241907199</v>
+        <v>0.26558264395501924</v>
       </c>
       <c r="J14" s="30">
-        <v>0.19444424313328701</v>
+        <v>0.2542796677646712</v>
+      </c>
+      <c r="K14" s="30">
+        <v>0.25565928356184919</v>
       </c>
       <c r="L14" s="30">
         <f t="shared" si="0"/>
-        <v>0.13734812058446252</v>
+        <v>0.17723840367205199</v>
       </c>
       <c r="M14" s="30">
         <v>2.3155875486813523E-2</v>
@@ -12742,17 +12778,20 @@
       </c>
       <c r="H15" s="31">
         <f>VLOOKUP(F15,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>4.2546573385120396</v>
+        <v>4.6984287524850101</v>
       </c>
       <c r="I15" s="30">
-        <v>4.4510147654637802</v>
+        <v>4.3090308460490396</v>
       </c>
       <c r="J15" s="30">
-        <v>4.5897245674903298</v>
+        <v>4.2602225832464828</v>
+      </c>
+      <c r="K15" s="30">
+        <v>4.1432118323518896</v>
       </c>
       <c r="L15" s="30">
         <f t="shared" si="0"/>
-        <v>4.1809760165229068</v>
+        <v>3.9613080270270089</v>
       </c>
       <c r="M15" s="30">
         <v>3.3634789145880619</v>
@@ -12778,17 +12817,20 @@
       </c>
       <c r="H16" s="31">
         <f>VLOOKUP(F16,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>4.0239683065477196</v>
+        <v>1.9571195447376</v>
       </c>
       <c r="I16" s="30">
-        <v>4.3602102234671296</v>
+        <v>2.1699504611733866</v>
       </c>
       <c r="J16" s="30">
-        <v>3.5251257971202601</v>
+        <v>1.9706387130131231</v>
+      </c>
+      <c r="K16" s="30">
+        <v>1.9076981609625141</v>
       </c>
       <c r="L16" s="30">
         <f t="shared" si="0"/>
-        <v>3.4314725583947805</v>
+        <v>2.3951478356566893</v>
       </c>
       <c r="M16" s="30">
         <v>3.2441660809438213</v>
@@ -12822,6 +12864,7 @@
       <c r="J17" s="30">
         <v>10.76129175</v>
       </c>
+      <c r="K17" s="30"/>
       <c r="L17" s="30">
         <v>16.798154247711324</v>
       </c>
@@ -12857,6 +12900,7 @@
       <c r="J18" s="30">
         <v>23.13677727</v>
       </c>
+      <c r="K18" s="30"/>
       <c r="L18" s="30">
         <v>30.018312954312446</v>
       </c>
@@ -12892,6 +12936,7 @@
       <c r="J19" s="30">
         <v>19.908389740000001</v>
       </c>
+      <c r="K19" s="30"/>
       <c r="L19" s="30">
         <v>25.857221286837778</v>
       </c>
@@ -12927,6 +12972,7 @@
       <c r="J20" s="30">
         <v>11.754512350000001</v>
       </c>
+      <c r="K20" s="30"/>
       <c r="L20" s="30">
         <f>(J20*2/3)+(M20/3)</f>
         <v>10.986341566666667</v>
@@ -12955,7 +13001,7 @@
       </c>
       <c r="H21" s="31">
         <f>VLOOKUP(F21,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>7.7245727925227703</v>
+        <v>7.7105748259750104</v>
       </c>
       <c r="I21" s="30">
         <v>10.927548</v>
@@ -12963,6 +13009,7 @@
       <c r="J21" s="30">
         <v>9.9341345454545458</v>
       </c>
+      <c r="K21" s="30"/>
       <c r="L21" s="30">
         <v>0</v>
       </c>
@@ -12998,6 +13045,7 @@
       <c r="J22" s="30">
         <v>4.4094344637268001</v>
       </c>
+      <c r="K22" s="30"/>
       <c r="L22" s="30">
         <f>(J22*2/3)+(M22/3)</f>
         <v>4.1107229120604369</v>
@@ -13027,7 +13075,7 @@
       </c>
       <c r="H23" s="31">
         <f>VLOOKUP(F23,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>21.784659175997099</v>
+        <v>20.831454920682301</v>
       </c>
       <c r="I23" s="30">
         <v>13.63038308</v>
@@ -13035,6 +13083,7 @@
       <c r="J23" s="30">
         <v>13.57977245</v>
       </c>
+      <c r="K23" s="30"/>
       <c r="L23" s="30">
         <v>0</v>
       </c>
@@ -13070,6 +13119,7 @@
       <c r="J24" s="30">
         <v>0.23</v>
       </c>
+      <c r="K24" s="30"/>
       <c r="L24" s="30">
         <f>(J24*2/3)+(M24/3)</f>
         <v>0.23116440009552636</v>
@@ -13099,7 +13149,7 @@
       </c>
       <c r="H25" s="31">
         <f>VLOOKUP(F25,'BY-Demands'!$I$6:$J$42,2,FALSE)</f>
-        <v>45.935836654432002</v>
+        <v>45.9683637522608</v>
       </c>
       <c r="I25" s="30">
         <v>46.104277330000002</v>
@@ -13107,13 +13157,14 @@
       <c r="J25" s="30">
         <v>46.814427170000002</v>
       </c>
+      <c r="K25" s="30"/>
       <c r="L25" s="30">
         <f>(J25*2/3)+(M25/3)</f>
-        <v>46.521563664810671</v>
+        <v>46.532406030753599</v>
       </c>
       <c r="M25" s="30">
         <f>H25</f>
-        <v>45.935836654432002</v>
+        <v>45.9683637522608</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -13144,6 +13195,7 @@
       <c r="J26" s="30">
         <v>29.618106901468909</v>
       </c>
+      <c r="K26" s="30"/>
       <c r="L26" s="30">
         <f>J26*2/3+M26*1/3</f>
         <v>30.669454951005577</v>
@@ -13179,6 +13231,7 @@
       <c r="J27" s="30">
         <v>59.593058464401295</v>
       </c>
+      <c r="K27" s="30"/>
       <c r="L27" s="30">
         <f>J27*2/3+M27*1/3</f>
         <v>61.758486976267527</v>
@@ -13209,10 +13262,10 @@
         <v>5.6291760000000002</v>
       </c>
       <c r="I28" s="31"/>
-      <c r="J28" s="1">
+      <c r="J28" s="31">
         <v>10.868399999999999</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="31">
         <v>14.3748</v>
       </c>
       <c r="L28" s="30">
@@ -13806,7 +13859,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C4:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update freight demand for 2019-2021 based on Eurostat
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABC998A-20E4-45CB-8462-66A71F45EAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E7D385-D7FE-451D-950F-C8E5518FADA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -147,6 +147,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9A259E39-3EDA-4082-BE12-276C248AF926}</author>
+    <author>tc={C162B4B5-5414-4E02-9B39-FB4FB193D264}</author>
+    <author>tc={A11FAA6D-9C88-4B20-8831-F494B83541E5}</author>
+  </authors>
+  <commentList>
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{9A259E39-3EDA-4082-BE12-276C248AF926}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="1" shapeId="0" xr:uid="{C162B4B5-5414-4E02-9B39-FB4FB193D264}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="2" shapeId="0" xr:uid="{A11FAA6D-9C88-4B20-8831-F494B83541E5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="203">
   <si>
@@ -787,7 +829,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -938,6 +980,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1600,6 +1648,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{60EFCDC4-4930-4B73-83DC-CF10A270283F}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1861,6 +1915,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H20" dT="2022-10-12T22:37:02.29" personId="{60EFCDC4-4930-4B73-83DC-CF10A270283F}" id="{9A259E39-3EDA-4082-BE12-276C248AF926}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+  <threadedComment ref="I20" dT="2022-10-12T22:37:46.05" personId="{60EFCDC4-4930-4B73-83DC-CF10A270283F}" id="{C162B4B5-5414-4E02-9B39-FB4FB193D264}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+  <threadedComment ref="J20" dT="2022-10-12T22:37:54.36" personId="{60EFCDC4-4930-4B73-83DC-CF10A270283F}" id="{A11FAA6D-9C88-4B20-8831-F494B83541E5}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CF3712-19CC-4E57-A353-BD088DDFAAD0}">
   <sheetPr codeName="Sheet7"/>
@@ -7150,8 +7224,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AF57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9389,107 +9463,107 @@
       </c>
       <c r="G22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2178146269505315</v>
+        <v>0.19157023231298867</v>
       </c>
       <c r="H22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.2532352952549441</v>
+        <v>2.8612543152225762</v>
       </c>
       <c r="I22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.59035591066396753</v>
+        <v>0.51922417028002199</v>
       </c>
       <c r="J22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37964907365901629</v>
+        <v>0.3339053132312666</v>
       </c>
       <c r="K22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2704057614094616</v>
+        <v>0.23782468265432868</v>
       </c>
       <c r="L22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.13049216248614431</v>
+        <v>0.11476921560539823</v>
       </c>
       <c r="M22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34195983528392676</v>
+        <v>0.30075723565585522</v>
       </c>
       <c r="N22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5291116374087359</v>
+        <v>0.4653591942698963</v>
       </c>
       <c r="O22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24890023926754198</v>
+        <v>0.21891035201263434</v>
       </c>
       <c r="P22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.28340932312027484</v>
+        <v>0.24926145057351232</v>
       </c>
       <c r="Q22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.57281742387914369</v>
+        <v>0.50379888854010457</v>
       </c>
       <c r="R22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3778873214697962</v>
+        <v>0.33235583383728884</v>
       </c>
       <c r="S22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37186096343983388</v>
+        <v>0.32705558920283034</v>
       </c>
       <c r="T22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.9896591411313085</v>
+        <v>1.7499259311761122</v>
       </c>
       <c r="U22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.54135919368811836</v>
+        <v>0.47613104754052427</v>
       </c>
       <c r="V22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.60997441370730043</v>
+        <v>0.53647884797665768</v>
       </c>
       <c r="W22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.49935221643128408</v>
+        <v>0.43918547366184335</v>
       </c>
       <c r="X22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46383071132724779</v>
+        <v>0.40794394006900198</v>
       </c>
       <c r="Y22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.74064511268734978</v>
+        <v>0.6514050882873873</v>
       </c>
       <c r="Z22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>9.8775540783756666E-2</v>
+        <v>8.6874116581173791E-2</v>
       </c>
       <c r="AA22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41714780682374364</v>
+        <v>0.36688583949060316</v>
       </c>
       <c r="AB22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18524594530412608</v>
+        <v>0.1629257376962582</v>
       </c>
       <c r="AC22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20201145503880613</v>
+        <v>0.17767117807225169</v>
       </c>
       <c r="AD22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.23481230791235341</v>
+        <v>0.20651986970064592</v>
       </c>
       <c r="AE22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.49070889678091939</v>
+        <v>0.43158358403414709</v>
       </c>
       <c r="AF22" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18922217409036649</v>
+        <v>0.16642287231469072</v>
       </c>
     </row>
     <row r="23" spans="4:32" x14ac:dyDescent="0.25">
@@ -9505,107 +9579,107 @@
       </c>
       <c r="G23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.17991488188042462</v>
+        <v>0.17598869695867239</v>
       </c>
       <c r="H23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>2.6871723541686299</v>
+        <v>2.6285316488038659</v>
       </c>
       <c r="I23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.48763398226070803</v>
+        <v>0.47699261024925638</v>
       </c>
       <c r="J23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3135901348759621</v>
+        <v>0.30674682738359726</v>
       </c>
       <c r="K23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22335515894815736</v>
+        <v>0.21848100041223001</v>
       </c>
       <c r="L23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.10778652622510916</v>
+        <v>0.10543435930256223</v>
       </c>
       <c r="M23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2824588239748011</v>
+        <v>0.27629487820158383</v>
       </c>
       <c r="N23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.43704621254646414</v>
+        <v>0.42750879000601366</v>
       </c>
       <c r="O23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20559159765702764</v>
+        <v>0.20110508368818067</v>
       </c>
       <c r="P23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.23409610092244049</v>
+        <v>0.22898754863328891</v>
       </c>
       <c r="Q23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47314719217489071</v>
+        <v>0.4628219575290925</v>
       </c>
       <c r="R23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.31213492756751032</v>
+        <v>0.30532337627525935</v>
       </c>
       <c r="S23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30715715583422787</v>
+        <v>0.30045423175568414</v>
       </c>
       <c r="T23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.643458450750628</v>
+        <v>1.6075941480235647</v>
       </c>
       <c r="U23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44716269403431846</v>
+        <v>0.4374045050032716</v>
       </c>
       <c r="V23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50383886577623815</v>
+        <v>0.4928438633777254</v>
       </c>
       <c r="W23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41246493081645397</v>
+        <v>0.40346393225981741</v>
       </c>
       <c r="X23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.38312416759737483</v>
+        <v>0.37476345660861177</v>
       </c>
       <c r="Y23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.61177286314532875</v>
+        <v>0.59842247564144924</v>
       </c>
       <c r="Z23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.1588596696128737E-2</v>
+        <v>7.9808132985805066E-2</v>
       </c>
       <c r="AA23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34456408847334713</v>
+        <v>0.33704485318495958</v>
       </c>
       <c r="AB23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.15301315083761008</v>
+        <v>0.14967402780693329</v>
       </c>
       <c r="AC23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.16686146187994025</v>
+        <v>0.16322013466560803</v>
       </c>
       <c r="AD23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.1939549663563945</v>
+        <v>0.18972239228331952</v>
       </c>
       <c r="AE23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.40532554878448751</v>
+        <v>0.39648034909113317</v>
       </c>
       <c r="AF23" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.15629751581539669</v>
+        <v>0.15288671986851338</v>
       </c>
     </row>
     <row r="24" spans="4:32" x14ac:dyDescent="0.25">
@@ -9621,107 +9695,107 @@
       </c>
       <c r="G24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.19572571146618054</v>
+        <v>0.19228961557590898</v>
       </c>
       <c r="H24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>2.9233197129377184</v>
+        <v>2.871998878406937</v>
       </c>
       <c r="I24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53048701205549609</v>
+        <v>0.52117395743271944</v>
       </c>
       <c r="J24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34114827865193581</v>
+        <v>0.33515919224388002</v>
       </c>
       <c r="K24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24298349829573737</v>
+        <v>0.23871776032169476</v>
       </c>
       <c r="L24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.11725875209088529</v>
+        <v>0.11520019620091229</v>
       </c>
       <c r="M24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30728116376227216</v>
+        <v>0.30188663722790898</v>
       </c>
       <c r="N24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47545361451038171</v>
+        <v>0.46710670802274745</v>
       </c>
       <c r="O24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22365888414741908</v>
+        <v>0.21973240271130756</v>
       </c>
       <c r="P24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.25466834886374512</v>
+        <v>0.25019747551574262</v>
       </c>
       <c r="Q24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.51472713012259241</v>
+        <v>0.50569075077735171</v>
       </c>
       <c r="R24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.33956518845505695</v>
+        <v>0.33360389425518211</v>
       </c>
       <c r="S24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3341499726383883</v>
+        <v>0.32828374617730566</v>
       </c>
       <c r="T24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.7878847551480515</v>
+        <v>1.7564972414002475</v>
       </c>
       <c r="U24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.48645912731760305</v>
+        <v>0.47791901168517154</v>
       </c>
       <c r="V24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.54811597260702893</v>
+        <v>0.53849342978034132</v>
       </c>
       <c r="W24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44871214207035037</v>
+        <v>0.44083470003305669</v>
       </c>
       <c r="X24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41679292729504486</v>
+        <v>0.40947584844094537</v>
       </c>
       <c r="Y24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.66553515553206655</v>
+        <v>0.65385124034471442</v>
       </c>
       <c r="Z24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.8758561654118218E-2</v>
+        <v>8.7200345686264502E-2</v>
       </c>
       <c r="AA24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37484420775688798</v>
+        <v>0.36826356675618782</v>
       </c>
       <c r="AB24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.16645986979152586</v>
+        <v>0.1635375553434078</v>
       </c>
       <c r="AC24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18152516346282133</v>
+        <v>0.17833836769908104</v>
       </c>
       <c r="AD24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21099963152428264</v>
+        <v>0.2072953917425068</v>
       </c>
       <c r="AE24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44094535472607599</v>
+        <v>0.43320426383996402</v>
       </c>
       <c r="AF24" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.17003286311633117</v>
+        <v>0.16704782237851226</v>
       </c>
     </row>
     <row r="25" spans="4:32" x14ac:dyDescent="0.25">
@@ -14322,12 +14396,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:AN42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14420,7 +14494,7 @@
         <v>1.7028384806625201</v>
       </c>
       <c r="L3" s="30">
-        <f t="shared" ref="L3:L19" si="0">K3*2/3+M3/3</f>
+        <f t="shared" ref="L3:L16" si="0">K3*2/3+M3/3</f>
         <v>1.1584060685789734</v>
       </c>
       <c r="M3" s="30">
@@ -15102,13 +15176,16 @@
         <v>11.625551</v>
       </c>
       <c r="H20" s="30">
-        <v>14.23064449</v>
+        <f>(12444+72)/1000</f>
+        <v>12.516</v>
       </c>
       <c r="I20" s="30">
-        <v>11.754512350000001</v>
+        <f>(11424+74)/1000</f>
+        <v>11.497999999999999</v>
       </c>
       <c r="J20" s="30">
-        <v>12.787492999999998</v>
+        <f>(12493+70)/1000</f>
+        <v>12.563000000000001</v>
       </c>
       <c r="K20" s="30">
         <v>13.183905282999998</v>
@@ -16020,6 +16097,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Include 2021 PKM adjustment
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E7D385-D7FE-451D-950F-C8E5518FADA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B530EADB-74B1-443E-A9B7-97D44E917CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="DEMANDS" sheetId="1" r:id="rId5"/>
     <sheet name="Residential" sheetId="8" r:id="rId6"/>
     <sheet name="Services" sheetId="9" r:id="rId7"/>
+    <sheet name="TRA-2021" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
@@ -54,26 +55,31 @@
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="I_alku">"1.1."</definedName>
     <definedName name="I_loppu">"31.3."</definedName>
@@ -123,11 +129,13 @@
     <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="1" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -150,12 +158,37 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>vahid Aryanpur</author>
     <author>tc={9A259E39-3EDA-4082-BE12-276C248AF926}</author>
     <author>tc={C162B4B5-5414-4E02-9B39-FB4FB193D264}</author>
     <author>tc={A11FAA6D-9C88-4B20-8831-F494B83541E5}</author>
   </authors>
   <commentList>
-    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{9A259E39-3EDA-4082-BE12-276C248AF926}">
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{A76B0409-052C-4EE2-A677-378739E63FB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>vahid Aryanpur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Updated, based on proportion of total fuel consumption</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="1" shapeId="0" xr:uid="{9A259E39-3EDA-4082-BE12-276C248AF926}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -165,7 +198,7 @@
 2) RAIL_GO_TOTAL</t>
       </text>
     </comment>
-    <comment ref="I20" authorId="1" shapeId="0" xr:uid="{C162B4B5-5414-4E02-9B39-FB4FB193D264}">
+    <comment ref="I20" authorId="2" shapeId="0" xr:uid="{C162B4B5-5414-4E02-9B39-FB4FB193D264}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -175,7 +208,7 @@
 2) RAIL_GO_TOTAL</t>
       </text>
     </comment>
-    <comment ref="J20" authorId="2" shapeId="0" xr:uid="{A11FAA6D-9C88-4B20-8831-F494B83541E5}">
+    <comment ref="J20" authorId="3" shapeId="0" xr:uid="{A11FAA6D-9C88-4B20-8831-F494B83541E5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -190,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="214">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -818,18 +851,52 @@
   <si>
     <t>RSDSH_Det*</t>
   </si>
+  <si>
+    <t>Total fuel consumption (litre)</t>
+  </si>
+  <si>
+    <t>6,681,011,455</t>
+  </si>
+  <si>
+    <t>6,688,720,344</t>
+  </si>
+  <si>
+    <t>6,132,509,241</t>
+  </si>
+  <si>
+    <t>6,231,032,199</t>
+  </si>
+  <si>
+    <t>Source: NORA (National Oil Reserves Agency), https://www.nora.ie/statistics.312.html</t>
+  </si>
+  <si>
+    <t>Proportion of total fuel consumption</t>
+  </si>
+  <si>
+    <t>ALL FUELS</t>
+  </si>
+  <si>
+    <t>2021/2018</t>
+  </si>
+  <si>
+    <t>2021/2020</t>
+  </si>
+  <si>
+    <t>Original value (2021)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,10 +1049,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1150,12 +1224,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1253,11 +1328,29 @@
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0CB343EE-8EF5-4039-B056-A39AE7D2D8C5}"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7224,7 +7317,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AF57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
@@ -7607,107 +7700,107 @@
       </c>
       <c r="G6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20300060063434958</v>
+        <v>0.17791021665128046</v>
       </c>
       <c r="H6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>4.0584633282751126</v>
+        <v>3.5568470622668977</v>
       </c>
       <c r="I6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.74848244469808678</v>
+        <v>0.65597182215127059</v>
       </c>
       <c r="J6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34724754504054051</v>
+        <v>0.30432858709155108</v>
       </c>
       <c r="K6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.27376982026764263</v>
+        <v>0.23993253164866168</v>
       </c>
       <c r="L6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.13755999795611623</v>
+        <v>0.12055791442215673</v>
       </c>
       <c r="M6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.39445499612536866</v>
+        <v>0.34570131123035525</v>
       </c>
       <c r="N6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.64928302501009705</v>
+        <v>0.56903321116577554</v>
       </c>
       <c r="O6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.26877256463954802</v>
+        <v>0.2355529247476085</v>
       </c>
       <c r="P6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30465079595834027</v>
+        <v>0.26699669332289716</v>
       </c>
       <c r="Q6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53022575007917072</v>
+        <v>0.46469112788778127</v>
       </c>
       <c r="R6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46901260006304341</v>
+        <v>0.41104377538121051</v>
       </c>
       <c r="S6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41278839282092511</v>
+        <v>0.36176874437029644</v>
       </c>
       <c r="T6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.7456271862846215</v>
+        <v>1.5298718818259087</v>
       </c>
       <c r="U6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53447019407874841</v>
+        <v>0.46841096885952921</v>
       </c>
       <c r="V6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.6373124074899349</v>
+        <v>0.5585421330615401</v>
       </c>
       <c r="W6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.58101868325410067</v>
+        <v>0.50920617718944683</v>
       </c>
       <c r="X6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.38581506771754165</v>
+        <v>0.33812925710793035</v>
       </c>
       <c r="Y6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.86232255454765427</v>
+        <v>0.75574156935227998</v>
       </c>
       <c r="Z6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.11067259735658087</v>
+        <v>9.699373160247457E-2</v>
       </c>
       <c r="AA6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46181565455091583</v>
+        <v>0.40473635495344346</v>
       </c>
       <c r="AB6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24158039942260146</v>
+        <v>0.21172164548120723</v>
       </c>
       <c r="AC6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21298903965802496</v>
+        <v>0.18666410873414702</v>
       </c>
       <c r="AD6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2375678491388247</v>
+        <v>0.2082050367220207</v>
       </c>
       <c r="AE6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46084064726442553</v>
+        <v>0.40388185621287809</v>
       </c>
       <c r="AF6" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22102568255169014</v>
+        <v>0.19370744197499956</v>
       </c>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
@@ -8303,107 +8396,107 @@
       </c>
       <c r="G12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46342451965761583</v>
+        <v>0.40588049118145847</v>
       </c>
       <c r="H12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.1155755961155194</v>
+        <v>7.107853964234006</v>
       </c>
       <c r="I12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.6525894242319275</v>
+        <v>1.4473852348686691</v>
       </c>
       <c r="J12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.7848468237617493</v>
+        <v>0.68739136756505304</v>
       </c>
       <c r="K12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.59049140670441203</v>
+        <v>0.51716931673940703</v>
       </c>
       <c r="L12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3042181315799129</v>
+        <v>0.26644296845403537</v>
       </c>
       <c r="M12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.81942741912586947</v>
+        <v>0.71767804519295675</v>
       </c>
       <c r="N12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.4226196661202095</v>
+        <v>1.2459711222787131</v>
       </c>
       <c r="O12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.60289301217975388</v>
+        <v>0.52803099864930969</v>
       </c>
       <c r="P12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.68057420745305641</v>
+        <v>0.59606641834696639</v>
       </c>
       <c r="Q12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2070161615941664</v>
+        <v>1.057139386784598</v>
       </c>
       <c r="R12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0242599623466919</v>
+        <v>0.89707626372882077</v>
       </c>
       <c r="S12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.9289528309484778</v>
+        <v>0.81360354343861541</v>
       </c>
       <c r="T12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.7541899081155736</v>
+        <v>3.2880272390856486</v>
       </c>
       <c r="U12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2287453474819043</v>
+        <v>1.0761704312524312</v>
       </c>
       <c r="V12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.3838834420094299</v>
+        <v>1.2120448257585934</v>
       </c>
       <c r="W12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.3422029707145537</v>
+        <v>1.1755398730764657</v>
       </c>
       <c r="X12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.84676500468112548</v>
+        <v>0.74162108700930296</v>
       </c>
       <c r="Y12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.8958558850984162</v>
+        <v>1.6604449812485407</v>
       </c>
       <c r="Z12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.248475056333125</v>
+        <v>0.21762158373782103</v>
       </c>
       <c r="AA12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0499837149519835</v>
+        <v>0.9196058643424867</v>
       </c>
       <c r="AB12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.56534360393881622</v>
+        <v>0.49514414952085861</v>
       </c>
       <c r="AC12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46120460967074761</v>
+        <v>0.40393623031991749</v>
       </c>
       <c r="AD12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50113203851603993</v>
+        <v>0.4389058181253126</v>
       </c>
       <c r="AE12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.92291572480430029</v>
+        <v>0.80831607265713046</v>
       </c>
       <c r="AF12" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50756865536512175</v>
+        <v>0.44454319184516294</v>
       </c>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.25">
@@ -8999,107 +9092,107 @@
       </c>
       <c r="G18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3949319127195085</v>
+        <v>0.34871475560546433</v>
       </c>
       <c r="H18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>7.0354598059455613</v>
+        <v>6.2121306680648631</v>
       </c>
       <c r="I18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.4215064973824205</v>
+        <v>1.2551537995825381</v>
       </c>
       <c r="J18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.68451237102108609</v>
+        <v>0.6044068774433683</v>
       </c>
       <c r="K18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5085872808789732</v>
+        <v>0.44906953235181829</v>
       </c>
       <c r="L18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2618778295465003</v>
+        <v>0.23123141075118878</v>
       </c>
       <c r="M18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.71158722914103401</v>
+        <v>0.62831328315096635</v>
       </c>
       <c r="N18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2100639919064762</v>
+        <v>1.0684554871723726</v>
       </c>
       <c r="O18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5215587975249425</v>
+        <v>0.46052304905013597</v>
       </c>
       <c r="P18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.57800689839391617</v>
+        <v>0.51036527517810415</v>
       </c>
       <c r="Q18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0273437110504584</v>
+        <v>0.90711816286219038</v>
       </c>
       <c r="R18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.87971877108373875</v>
+        <v>0.77676912495517314</v>
       </c>
       <c r="S18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.78875759816931479</v>
+        <v>0.69645274088780662</v>
       </c>
       <c r="T18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.2162421821708547</v>
+        <v>2.8398594046266692</v>
       </c>
       <c r="U18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0696076988780558</v>
+        <v>0.94443618075729097</v>
       </c>
       <c r="V18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.1848865981492651</v>
+        <v>1.0462244938591938</v>
       </c>
       <c r="W18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.1462954859601473</v>
+        <v>1.0121495310057134</v>
       </c>
       <c r="X18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.72187705815118308</v>
+        <v>0.63739893840679929</v>
       </c>
       <c r="Y18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.6400933547220824</v>
+        <v>1.4481603915565415</v>
       </c>
       <c r="Z18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21158507026178613</v>
+        <v>0.18682419346168758</v>
       </c>
       <c r="AA18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.90946181001663118</v>
+        <v>0.80303146592687813</v>
       </c>
       <c r="AB18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47670587805089104</v>
+        <v>0.42091907087353819</v>
       </c>
       <c r="AC18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.39733782511006455</v>
+        <v>0.35083911457535288</v>
       </c>
       <c r="AD18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.42495116243643605</v>
+        <v>0.37522098361933615</v>
       </c>
       <c r="AE18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.78279105429979845</v>
+        <v>0.69118443559198872</v>
       </c>
       <c r="AF18" s="13">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CN$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.45217630306421169</v>
+        <v>0.39926008492914083</v>
       </c>
     </row>
     <row r="19" spans="4:32" x14ac:dyDescent="0.25">
@@ -14400,8 +14493,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:AN42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15061,8 +15154,9 @@
       <c r="I17" s="30">
         <v>10.76129175</v>
       </c>
-      <c r="J17" s="30">
-        <v>15.490769824884</v>
+      <c r="J17" s="1">
+        <f>G17*'TRA-2021'!$C$11</f>
+        <v>13.576148085415543</v>
       </c>
       <c r="K17" s="30">
         <v>15.7055907873725</v>
@@ -15101,8 +15195,9 @@
       <c r="I18" s="30">
         <v>23.13677727</v>
       </c>
-      <c r="J18" s="30">
-        <v>33.305155123500498</v>
+      <c r="J18" s="1">
+        <f>G18*'TRA-2021'!$C$11</f>
+        <v>29.169610469442279</v>
       </c>
       <c r="K18" s="30">
         <v>33.767020192851</v>
@@ -15141,8 +15236,9 @@
       <c r="I19" s="30">
         <v>19.908389740000001</v>
       </c>
-      <c r="J19" s="30">
-        <v>28.657924176035301</v>
+      <c r="J19" s="1">
+        <f>G19*'TRA-2021'!$C$11</f>
+        <v>25.304212456246088</v>
       </c>
       <c r="K19" s="30">
         <v>29.055342956639201</v>
@@ -17790,4 +17886,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5796510-5576-4C29-A9D1-EA490DE360B3}">
+  <dimension ref="B2:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="51">
+        <v>2018</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="51">
+        <v>2019</v>
+      </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="51">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="52">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="54">
+        <f>C6/C3</f>
+        <v>0.93264803405429875</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="55">
+        <f>C6/C5</f>
+        <v>1.0160656843925007</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2018</v>
+      </c>
+      <c r="D16">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="56">
+        <v>14.5565610923972</v>
+      </c>
+      <c r="D17" s="56">
+        <v>15.490769824884</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="56">
+        <v>31.276118540281001</v>
+      </c>
+      <c r="D18" s="56">
+        <v>33.305155123500498</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="56">
+        <v>27.131577542973599</v>
+      </c>
+      <c r="D19" s="56">
+        <v>28.657924176035301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change DC demand projection according to GCS 2022 (medium)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABC998A-20E4-45CB-8462-66A71F45EAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ECBAE4-A617-4586-ADDD-AD6E3E0427F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -14327,7 +14327,7 @@
   <dimension ref="B1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14420,7 +14420,7 @@
         <v>1.7028384806625201</v>
       </c>
       <c r="L3" s="30">
-        <f t="shared" ref="L3:L19" si="0">K3*2/3+M3/3</f>
+        <f t="shared" ref="L3:L16" si="0">K3*2/3+M3/3</f>
         <v>1.1584060685789734</v>
       </c>
       <c r="M3" s="30">
@@ -15439,7 +15439,8 @@
         <v>14.3748</v>
       </c>
       <c r="K28" s="31">
-        <v>17.1311</v>
+        <f>600*8760/10^6*3.6</f>
+        <v>18.921600000000002</v>
       </c>
       <c r="L28" s="30">
         <v>25</v>

</xml_diff>

<commit_message>
Use medium demand projection from GCS 2022 for DCs in LED
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F42EEB-5B5C-4F01-83E1-CE4CF575DB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CAB61C-1D87-4E0A-9976-4B8B94FEE4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -14494,7 +14494,7 @@
   <dimension ref="B1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14507,7 +14507,7 @@
     <col min="7" max="40" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>146</v>
       </c>
@@ -14515,7 +14515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
@@ -14550,13 +14550,16 @@
         <v>2030</v>
       </c>
       <c r="M2" s="12">
+        <v>2031</v>
+      </c>
+      <c r="N2" s="12">
         <v>2050</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>59</v>
       </c>
@@ -14587,17 +14590,17 @@
         <v>1.7028384806625201</v>
       </c>
       <c r="L3" s="30">
-        <f t="shared" ref="L3:L16" si="0">K3*2/3+M3/3</f>
+        <f>K3*2/3+N3/3</f>
         <v>1.1584060685789734</v>
       </c>
-      <c r="M3" s="30">
+      <c r="N3" s="30">
         <v>6.9541244411880462E-2</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>59</v>
       </c>
@@ -14628,17 +14631,17 @@
         <v>23.738094411807602</v>
       </c>
       <c r="L4" s="30">
-        <f t="shared" si="0"/>
+        <f>K4*2/3+N4/3</f>
         <v>22.05783877515594</v>
       </c>
-      <c r="M4" s="30">
+      <c r="N4" s="30">
         <v>18.697327501852616</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>59</v>
       </c>
@@ -14669,17 +14672,17 @@
         <v>1.5478463345837199</v>
       </c>
       <c r="L5" s="30">
-        <f t="shared" si="0"/>
+        <f>K5*2/3+N5/3</f>
         <v>1.9434753073389506</v>
       </c>
-      <c r="M5" s="30">
+      <c r="N5" s="30">
         <v>2.7347332528494115</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>59</v>
       </c>
@@ -14710,17 +14713,17 @@
         <v>5.8166390635502099</v>
       </c>
       <c r="L6" s="30">
-        <f t="shared" si="0"/>
+        <f>K6*2/3+N6/3</f>
         <v>5.2807562869892761</v>
       </c>
-      <c r="M6" s="30">
+      <c r="N6" s="30">
         <v>4.2089907338674086</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>59</v>
       </c>
@@ -14751,17 +14754,17 @@
         <v>1.19927927754182</v>
       </c>
       <c r="L7" s="30">
-        <f t="shared" si="0"/>
+        <f>K7*2/3+N7/3</f>
         <v>1.22325956804396</v>
       </c>
-      <c r="M7" s="30">
+      <c r="N7" s="30">
         <v>1.2712201490482398</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>59</v>
       </c>
@@ -14792,17 +14795,17 @@
         <v>10.6043548094603</v>
       </c>
       <c r="L8" s="30">
-        <f t="shared" si="0"/>
+        <f>K8*2/3+N8/3</f>
         <v>9.4725222533350699</v>
       </c>
-      <c r="M8" s="30">
+      <c r="N8" s="30">
         <v>7.2088571410846098</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>59</v>
       </c>
@@ -14833,17 +14836,17 @@
         <v>1.0410295169864401</v>
       </c>
       <c r="L9" s="30">
-        <f t="shared" si="0"/>
+        <f>K9*2/3+N9/3</f>
         <v>0.85675812345956381</v>
       </c>
-      <c r="M9" s="30">
+      <c r="N9" s="30">
         <v>0.48821533640581133</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>59</v>
       </c>
@@ -14874,17 +14877,17 @@
         <v>18.752348682008719</v>
       </c>
       <c r="L10" s="30">
-        <f t="shared" si="0"/>
+        <f>K10*2/3+N10/3</f>
         <v>15.463248848798345</v>
       </c>
-      <c r="M10" s="30">
+      <c r="N10" s="30">
         <v>8.8850491823775997</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>59</v>
       </c>
@@ -14915,17 +14918,17 @@
         <v>18.095637208589601</v>
       </c>
       <c r="L11" s="30">
-        <f t="shared" si="0"/>
+        <f>K11*2/3+N11/3</f>
         <v>16.048363755990756</v>
       </c>
-      <c r="M11" s="30">
+      <c r="N11" s="30">
         <v>11.953816850793071</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>59</v>
       </c>
@@ -14956,17 +14959,17 @@
         <v>2.2584342466232901</v>
       </c>
       <c r="L12" s="30">
-        <f t="shared" si="0"/>
+        <f>K12*2/3+N12/3</f>
         <v>1.8148484316492632</v>
       </c>
-      <c r="M12" s="30">
+      <c r="N12" s="30">
         <v>0.92767680170120992</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>59</v>
       </c>
@@ -14997,17 +15000,17 @@
         <v>6.2862087424890802</v>
       </c>
       <c r="L13" s="30">
-        <f t="shared" si="0"/>
+        <f>K13*2/3+N13/3</f>
         <v>7.1919298250215675</v>
       </c>
-      <c r="M13" s="30">
+      <c r="N13" s="30">
         <v>9.0033719900865421</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>59</v>
       </c>
@@ -15038,17 +15041,17 @@
         <v>0.187409320968947</v>
       </c>
       <c r="L14" s="30">
-        <f t="shared" si="0"/>
+        <f>K14*2/3+N14/3</f>
         <v>0.1326581724749025</v>
       </c>
-      <c r="M14" s="30">
+      <c r="N14" s="30">
         <v>2.3155875486813523E-2</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>59</v>
       </c>
@@ -15079,17 +15082,17 @@
         <v>4.6924479738735299</v>
       </c>
       <c r="L15" s="30">
-        <f t="shared" si="0"/>
+        <f>K15*2/3+N15/3</f>
         <v>4.2494582874450408</v>
       </c>
-      <c r="M15" s="30">
+      <c r="N15" s="30">
         <v>3.3634789145880619</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>59</v>
       </c>
@@ -15120,17 +15123,17 @@
         <v>3.6347440465271599</v>
       </c>
       <c r="L16" s="30">
-        <f t="shared" si="0"/>
+        <f>K16*2/3+N16/3</f>
         <v>3.5045513913327135</v>
       </c>
-      <c r="M16" s="30">
+      <c r="N16" s="30">
         <v>3.2441660809438213</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>59</v>
       </c>
@@ -15164,14 +15167,14 @@
       <c r="L17" s="30">
         <v>16.798154247711324</v>
       </c>
-      <c r="M17" s="30">
+      <c r="N17" s="30">
         <v>18.550648173612263</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>59</v>
       </c>
@@ -15205,14 +15208,14 @@
       <c r="L18" s="30">
         <v>30.018312954312446</v>
       </c>
-      <c r="M18" s="30">
+      <c r="N18" s="30">
         <v>30.011573675084005</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>59</v>
       </c>
@@ -15246,14 +15249,14 @@
       <c r="L19" s="30">
         <v>25.857221286837778</v>
       </c>
-      <c r="M19" s="30">
+      <c r="N19" s="30">
         <v>25.788290151303741</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>59</v>
       </c>
@@ -15287,17 +15290,17 @@
         <v>13.183905282999998</v>
       </c>
       <c r="L20" s="30">
-        <f>K20*2/3+M20/3</f>
+        <f>K20*2/3+N20/3</f>
         <v>11.939270188666665</v>
       </c>
-      <c r="M20" s="30">
+      <c r="N20" s="30">
         <v>9.4499999999999993</v>
       </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>59</v>
       </c>
@@ -15325,20 +15328,20 @@
         <v>8.6157094085103783</v>
       </c>
       <c r="K21" s="30">
-        <f t="shared" ref="K21" si="1">J21-($H$21/11)</f>
+        <f t="shared" ref="K21" si="0">J21-($H$21/11)</f>
         <v>7.6814227047944605</v>
       </c>
       <c r="L21" s="30">
         <v>0</v>
       </c>
-      <c r="M21" s="30">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="30">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>59</v>
       </c>
@@ -15369,18 +15372,18 @@
         <v>4.6611834502685596</v>
       </c>
       <c r="L22" s="30">
-        <f>K22*2/3+M22/3</f>
+        <f>K22*2/3+N22/3</f>
         <v>4.2785555697549427</v>
       </c>
-      <c r="M22" s="30">
+      <c r="N22" s="30">
         <f>G22</f>
         <v>3.5132998087277101</v>
       </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>59</v>
       </c>
@@ -15413,14 +15416,14 @@
       <c r="L23" s="30">
         <v>0</v>
       </c>
-      <c r="M23" s="30">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="30">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>59</v>
       </c>
@@ -15451,18 +15454,18 @@
         <v>0.23</v>
       </c>
       <c r="L24" s="30">
-        <f>K24*2/3+M24/3</f>
+        <f>K24*2/3+N24/3</f>
         <v>0.23116440009552636</v>
       </c>
-      <c r="M24" s="30">
+      <c r="N24" s="30">
         <f>G24</f>
         <v>0.23349320028657899</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>59</v>
       </c>
@@ -15493,18 +15496,18 @@
         <v>48.192396850000002</v>
       </c>
       <c r="L25" s="30">
-        <f>K25*2/3+M25/3</f>
+        <f>K25*2/3+N25/3</f>
         <v>47.451052484086929</v>
       </c>
-      <c r="M25" s="30">
+      <c r="N25" s="30">
         <f>G25</f>
         <v>45.9683637522608</v>
       </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>59</v>
       </c>
@@ -15535,17 +15538,17 @@
         <v>31.598021694557708</v>
       </c>
       <c r="L26" s="30">
-        <f>K26*2/3+M26/3</f>
+        <f>K26*2/3+N26/3</f>
         <v>31.989398146398109</v>
       </c>
-      <c r="M26" s="30">
+      <c r="N26" s="30">
         <v>32.772151050078904</v>
       </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>59</v>
       </c>
@@ -15576,17 +15579,17 @@
         <v>63.576742445676345</v>
       </c>
       <c r="L27" s="30">
-        <f>K27*2/3+M27/3</f>
+        <f>K27*2/3+N27/3</f>
         <v>64.414276297117567</v>
       </c>
-      <c r="M27" s="30">
+      <c r="N27" s="30">
         <v>66.089343999999997</v>
       </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>59</v>
       </c>
@@ -15615,17 +15618,20 @@
         <f>600*8760/10^6*3.6</f>
         <v>18.921600000000002</v>
       </c>
-      <c r="L28" s="30">
-        <v>25</v>
-      </c>
-      <c r="M28" s="30">
-        <v>30</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L28" s="30"/>
+      <c r="M28" s="31">
+        <f>1491*8760/10^6*3.6</f>
+        <v>47.020175999999999</v>
+      </c>
+      <c r="N28" s="30">
+        <f>M28</f>
+        <v>47.020175999999999</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>59</v>
       </c>
@@ -15650,24 +15656,24 @@
       <c r="L29" s="31">
         <v>0.5</v>
       </c>
-      <c r="M29" s="30">
+      <c r="N29" s="30">
         <v>0.54</v>
       </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>146</v>
       </c>

</xml_diff>